<commit_message>
11 tracking 04.10.21 10:18
</commit_message>
<xml_diff>
--- a/volumeTracker.xlsx
+++ b/volumeTracker.xlsx
@@ -1350,13 +1350,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K335"/>
+  <dimension ref="A1:L335"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1390,8 +1390,11 @@
       <c r="K1">
         <v>1176078971.051334</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1">
+        <v>1599333865.375042</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1425,8 +1428,11 @@
       <c r="K2">
         <v>1177692293.096379</v>
       </c>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="L2">
+        <v>1233300506.651645</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1460,8 +1466,11 @@
       <c r="K3">
         <v>352383755.2762</v>
       </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="L3">
+        <v>374992014.512</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1495,8 +1504,11 @@
       <c r="K4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="L4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1530,8 +1542,11 @@
       <c r="K5">
         <v>31190608.3499</v>
       </c>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="L5">
+        <v>34387215.8525</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1565,8 +1580,11 @@
       <c r="K6">
         <v>64045595.4849</v>
       </c>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="L6">
+        <v>73828981.9237</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1600,8 +1618,11 @@
       <c r="K7">
         <v>104753512.358</v>
       </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="L7">
+        <v>74257540.9761</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1635,8 +1656,11 @@
       <c r="K8">
         <v>280859164.8545</v>
       </c>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="L8">
+        <v>332842051.3593</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1670,8 +1694,11 @@
       <c r="K9">
         <v>421460115.7852</v>
       </c>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="L9">
+        <v>440925189.3433</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1705,8 +1732,11 @@
       <c r="K10">
         <v>136338891.4936</v>
       </c>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="L10">
+        <v>164579511.2285</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1740,8 +1770,11 @@
       <c r="K11">
         <v>3093789.115</v>
       </c>
-    </row>
-    <row r="12" spans="1:11">
+      <c r="L11">
+        <v>4125027.3291</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1775,8 +1808,11 @@
       <c r="K12">
         <v>44008100.6682</v>
       </c>
-    </row>
-    <row r="13" spans="1:11">
+      <c r="L12">
+        <v>41380425.3261</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1810,8 +1846,11 @@
       <c r="K13">
         <v>57928109.8876</v>
       </c>
-    </row>
-    <row r="14" spans="1:11">
+      <c r="L13">
+        <v>45639327.3091</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1845,8 +1884,11 @@
       <c r="K14">
         <v>26789845.8736</v>
       </c>
-    </row>
-    <row r="15" spans="1:11">
+      <c r="L14">
+        <v>32471220.1022</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1880,8 +1922,11 @@
       <c r="K15">
         <v>63641578.265353</v>
       </c>
-    </row>
-    <row r="16" spans="1:11">
+      <c r="L15">
+        <v>69216810.727956</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1915,8 +1960,11 @@
       <c r="K16">
         <v>80984118.79350001</v>
       </c>
-    </row>
-    <row r="17" spans="1:11">
+      <c r="L16">
+        <v>88729691.8444</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1950,8 +1998,11 @@
       <c r="K17">
         <v>47447395.749538</v>
       </c>
-    </row>
-    <row r="18" spans="1:11">
+      <c r="L17">
+        <v>43079030.049943</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1985,8 +2036,11 @@
       <c r="K18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:11">
+      <c r="L18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -2020,8 +2074,11 @@
       <c r="K19">
         <v>1506466.1709</v>
       </c>
-    </row>
-    <row r="20" spans="1:11">
+      <c r="L19">
+        <v>1210642.2615</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -2055,8 +2112,11 @@
       <c r="K20">
         <v>93765316.731181</v>
       </c>
-    </row>
-    <row r="21" spans="1:11">
+      <c r="L20">
+        <v>97777423.64961401</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -2090,8 +2150,11 @@
       <c r="K21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:11">
+      <c r="L21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -2125,8 +2188,11 @@
       <c r="K22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:11">
+      <c r="L22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -2160,8 +2226,11 @@
       <c r="K23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:11">
+      <c r="L23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -2195,8 +2264,11 @@
       <c r="K24">
         <v>104589607.3825</v>
       </c>
-    </row>
-    <row r="25" spans="1:11">
+      <c r="L24">
+        <v>88583153.4005</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -2230,8 +2302,11 @@
       <c r="K25">
         <v>109886806.2324</v>
       </c>
-    </row>
-    <row r="26" spans="1:11">
+      <c r="L25">
+        <v>130294006.4593</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -2265,8 +2340,11 @@
       <c r="K26">
         <v>15328499.0393</v>
       </c>
-    </row>
-    <row r="27" spans="1:11">
+      <c r="L26">
+        <v>12123957.1628</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -2300,8 +2378,11 @@
       <c r="K27">
         <v>21242400.783094</v>
       </c>
-    </row>
-    <row r="28" spans="1:11">
+      <c r="L27">
+        <v>33842824.899636</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -2335,8 +2416,11 @@
       <c r="K28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:11">
+      <c r="L28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -2370,8 +2454,11 @@
       <c r="K29">
         <v>3063767.3231</v>
       </c>
-    </row>
-    <row r="30" spans="1:11">
+      <c r="L29">
+        <v>3059302.7594</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -2405,8 +2492,11 @@
       <c r="K30">
         <v>20478552.767661</v>
       </c>
-    </row>
-    <row r="31" spans="1:11">
+      <c r="L30">
+        <v>50853421.449432</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -2440,8 +2530,11 @@
       <c r="K31">
         <v>20608691.784853</v>
       </c>
-    </row>
-    <row r="32" spans="1:11">
+      <c r="L31">
+        <v>18014715.183145</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -2475,8 +2568,11 @@
       <c r="K32">
         <v>5730817.9499</v>
       </c>
-    </row>
-    <row r="33" spans="1:11">
+      <c r="L32">
+        <v>5889939.6644</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -2510,8 +2606,11 @@
       <c r="K33">
         <v>102894324.2803</v>
       </c>
-    </row>
-    <row r="34" spans="1:11">
+      <c r="L33">
+        <v>119173580.8564</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -2545,8 +2644,11 @@
       <c r="K34">
         <v>8617403.696</v>
       </c>
-    </row>
-    <row r="35" spans="1:11">
+      <c r="L34">
+        <v>8455566.0558</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -2580,8 +2682,11 @@
       <c r="K35">
         <v>23396134.3687</v>
       </c>
-    </row>
-    <row r="36" spans="1:11">
+      <c r="L35">
+        <v>23617210.3725</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -2615,8 +2720,11 @@
       <c r="K36">
         <v>17193728.8807</v>
       </c>
-    </row>
-    <row r="37" spans="1:11">
+      <c r="L36">
+        <v>20703166.5804</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -2650,8 +2758,11 @@
       <c r="K37">
         <v>33132729.64992</v>
       </c>
-    </row>
-    <row r="38" spans="1:11">
+      <c r="L37">
+        <v>33440649.99499</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -2685,8 +2796,11 @@
       <c r="K38">
         <v>58237883.975797</v>
       </c>
-    </row>
-    <row r="39" spans="1:11">
+      <c r="L38">
+        <v>93655629.620315</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -2720,8 +2834,11 @@
       <c r="K39">
         <v>18900117.6575</v>
       </c>
-    </row>
-    <row r="40" spans="1:11">
+      <c r="L39">
+        <v>20245643.4723</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -2755,8 +2872,11 @@
       <c r="K40">
         <v>15431900.5572</v>
       </c>
-    </row>
-    <row r="41" spans="1:11">
+      <c r="L40">
+        <v>32591798.5157</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -2790,8 +2910,11 @@
       <c r="K41">
         <v>454830752.653364</v>
       </c>
-    </row>
-    <row r="42" spans="1:11">
+      <c r="L41">
+        <v>319594577.8478</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -2825,8 +2948,11 @@
       <c r="K42">
         <v>80487071.6532</v>
       </c>
-    </row>
-    <row r="43" spans="1:11">
+      <c r="L42">
+        <v>85571885.78910001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -2860,8 +2986,11 @@
       <c r="K43">
         <v>14785747.6105</v>
       </c>
-    </row>
-    <row r="44" spans="1:11">
+      <c r="L43">
+        <v>28768922.1361</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -2895,8 +3024,11 @@
       <c r="K44">
         <v>2810162.806891</v>
       </c>
-    </row>
-    <row r="45" spans="1:11">
+      <c r="L44">
+        <v>1970790.543664</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -2930,8 +3062,11 @@
       <c r="K45">
         <v>144012755.9798</v>
       </c>
-    </row>
-    <row r="46" spans="1:11">
+      <c r="L45">
+        <v>147497737.961</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -2965,8 +3100,11 @@
       <c r="K46">
         <v>148806385.1355</v>
       </c>
-    </row>
-    <row r="47" spans="1:11">
+      <c r="L46">
+        <v>126907980.6723</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -3000,8 +3138,11 @@
       <c r="K47">
         <v>13405909.5114</v>
       </c>
-    </row>
-    <row r="48" spans="1:11">
+      <c r="L47">
+        <v>7932188.8563</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -3035,8 +3176,11 @@
       <c r="K48">
         <v>64915974.982495</v>
       </c>
-    </row>
-    <row r="49" spans="1:11">
+      <c r="L48">
+        <v>89348518.803058</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -3070,8 +3214,11 @@
       <c r="K49">
         <v>232486491.5212</v>
       </c>
-    </row>
-    <row r="50" spans="1:11">
+      <c r="L49">
+        <v>213186255.6204</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -3105,8 +3252,11 @@
       <c r="K50">
         <v>130478030.9481</v>
       </c>
-    </row>
-    <row r="51" spans="1:11">
+      <c r="L50">
+        <v>243170993.5206</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -3140,8 +3290,11 @@
       <c r="K51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:11">
+      <c r="L51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -3175,8 +3328,11 @@
       <c r="K52">
         <v>2652423.170926</v>
       </c>
-    </row>
-    <row r="53" spans="1:11">
+      <c r="L52">
+        <v>1858190.187066</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -3210,8 +3366,11 @@
       <c r="K53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:11">
+      <c r="L53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -3245,8 +3404,11 @@
       <c r="K54">
         <v>132888055.3731</v>
       </c>
-    </row>
-    <row r="55" spans="1:11">
+      <c r="L54">
+        <v>212625344.682</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -3280,8 +3442,11 @@
       <c r="K55">
         <v>2001172.5013</v>
       </c>
-    </row>
-    <row r="56" spans="1:11">
+      <c r="L55">
+        <v>1323791.5346</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -3315,8 +3480,11 @@
       <c r="K56">
         <v>6390148.412433</v>
       </c>
-    </row>
-    <row r="57" spans="1:11">
+      <c r="L56">
+        <v>5378310.89414</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -3350,8 +3518,11 @@
       <c r="K57">
         <v>20894338.224289</v>
       </c>
-    </row>
-    <row r="58" spans="1:11">
+      <c r="L57">
+        <v>18280447.1672866</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -3385,8 +3556,11 @@
       <c r="K58">
         <v>3555429.874291</v>
       </c>
-    </row>
-    <row r="59" spans="1:11">
+      <c r="L58">
+        <v>4423998.407108</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -3420,8 +3594,11 @@
       <c r="K59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:11">
+      <c r="L59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -3455,8 +3632,11 @@
       <c r="K60">
         <v>1878275.4335</v>
       </c>
-    </row>
-    <row r="61" spans="1:11">
+      <c r="L60">
+        <v>1931966.0608</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -3490,8 +3670,11 @@
       <c r="K61">
         <v>7615363.9856</v>
       </c>
-    </row>
-    <row r="62" spans="1:11">
+      <c r="L61">
+        <v>11917869.0721</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -3525,8 +3708,11 @@
       <c r="K62">
         <v>5960441.35</v>
       </c>
-    </row>
-    <row r="63" spans="1:11">
+      <c r="L62">
+        <v>6280817.4596</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -3560,8 +3746,11 @@
       <c r="K63">
         <v>2793942.813231</v>
       </c>
-    </row>
-    <row r="64" spans="1:11">
+      <c r="L63">
+        <v>1749049.111837</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -3595,8 +3784,11 @@
       <c r="K64">
         <v>120308249.305663</v>
       </c>
-    </row>
-    <row r="65" spans="1:11">
+      <c r="L64">
+        <v>76901043.285624</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -3630,8 +3822,11 @@
       <c r="K65">
         <v>1394095.56986</v>
       </c>
-    </row>
-    <row r="66" spans="1:11">
+      <c r="L65">
+        <v>1053134.932202</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12">
       <c r="A66" t="s">
         <v>65</v>
       </c>
@@ -3665,8 +3860,11 @@
       <c r="K66">
         <v>2692262.283869</v>
       </c>
-    </row>
-    <row r="67" spans="1:11">
+      <c r="L66">
+        <v>2315799.128795</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12">
       <c r="A67" t="s">
         <v>66</v>
       </c>
@@ -3700,8 +3898,11 @@
       <c r="K67">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:11">
+      <c r="L67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -3735,8 +3936,11 @@
       <c r="K68">
         <v>8088704.03801</v>
       </c>
-    </row>
-    <row r="69" spans="1:11">
+      <c r="L68">
+        <v>5322013.31682</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -3770,8 +3974,11 @@
       <c r="K69">
         <v>2612386.7619</v>
       </c>
-    </row>
-    <row r="70" spans="1:11">
+      <c r="L69">
+        <v>3013214.6073</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12">
       <c r="A70" t="s">
         <v>69</v>
       </c>
@@ -3805,8 +4012,11 @@
       <c r="K70">
         <v>17069329.67545</v>
       </c>
-    </row>
-    <row r="71" spans="1:11">
+      <c r="L70">
+        <v>18559933.84047</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12">
       <c r="A71" t="s">
         <v>70</v>
       </c>
@@ -3840,8 +4050,11 @@
       <c r="K71">
         <v>19907875.0282</v>
       </c>
-    </row>
-    <row r="72" spans="1:11">
+      <c r="L71">
+        <v>17064727.3493</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12">
       <c r="A72" t="s">
         <v>71</v>
       </c>
@@ -3875,8 +4088,11 @@
       <c r="K72">
         <v>34278697.1154</v>
       </c>
-    </row>
-    <row r="73" spans="1:11">
+      <c r="L72">
+        <v>37655233.6835</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -3910,8 +4126,11 @@
       <c r="K73">
         <v>5928832.9386</v>
       </c>
-    </row>
-    <row r="74" spans="1:11">
+      <c r="L73">
+        <v>5314525.9905</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12">
       <c r="A74" t="s">
         <v>73</v>
       </c>
@@ -3945,8 +4164,11 @@
       <c r="K74">
         <v>540248233.7029999</v>
       </c>
-    </row>
-    <row r="75" spans="1:11">
+      <c r="L74">
+        <v>675012723.7740999</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12">
       <c r="A75" t="s">
         <v>74</v>
       </c>
@@ -3980,8 +4202,11 @@
       <c r="K75">
         <v>2947282.063</v>
       </c>
-    </row>
-    <row r="76" spans="1:11">
+      <c r="L75">
+        <v>3591488.2562</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12">
       <c r="A76" t="s">
         <v>75</v>
       </c>
@@ -4015,8 +4240,11 @@
       <c r="K76">
         <v>301860475.659519</v>
       </c>
-    </row>
-    <row r="77" spans="1:11">
+      <c r="L76">
+        <v>300854957.271232</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -4050,8 +4278,11 @@
       <c r="K77">
         <v>44381246.335141</v>
       </c>
-    </row>
-    <row r="78" spans="1:11">
+      <c r="L77">
+        <v>24212017.3147</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12">
       <c r="A78" t="s">
         <v>77</v>
       </c>
@@ -4085,8 +4316,11 @@
       <c r="K78">
         <v>12857092.155223</v>
       </c>
-    </row>
-    <row r="79" spans="1:11">
+      <c r="L78">
+        <v>10253174.766581</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12">
       <c r="A79" t="s">
         <v>78</v>
       </c>
@@ -4120,8 +4354,11 @@
       <c r="K79">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:11">
+      <c r="L79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12">
       <c r="A80" t="s">
         <v>79</v>
       </c>
@@ -4155,8 +4392,11 @@
       <c r="K80">
         <v>59540784.4526</v>
       </c>
-    </row>
-    <row r="81" spans="1:11">
+      <c r="L80">
+        <v>50508462.5668</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -4190,8 +4430,11 @@
       <c r="K81">
         <v>4666131.6306</v>
       </c>
-    </row>
-    <row r="82" spans="1:11">
+      <c r="L81">
+        <v>6815192.9747</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12">
       <c r="A82" t="s">
         <v>81</v>
       </c>
@@ -4225,8 +4468,11 @@
       <c r="K82">
         <v>2622089.8215</v>
       </c>
-    </row>
-    <row r="83" spans="1:11">
+      <c r="L82">
+        <v>2539386.0439</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12">
       <c r="A83" t="s">
         <v>82</v>
       </c>
@@ -4260,8 +4506,11 @@
       <c r="K83">
         <v>67253544.4149</v>
       </c>
-    </row>
-    <row r="84" spans="1:11">
+      <c r="L83">
+        <v>72863580.2509</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12">
       <c r="A84" t="s">
         <v>83</v>
       </c>
@@ -4295,8 +4544,11 @@
       <c r="K84">
         <v>11469527.144019</v>
       </c>
-    </row>
-    <row r="85" spans="1:11">
+      <c r="L84">
+        <v>14134578.832357</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12">
       <c r="A85" t="s">
         <v>84</v>
       </c>
@@ -4330,8 +4582,11 @@
       <c r="K85">
         <v>12000905.3017</v>
       </c>
-    </row>
-    <row r="86" spans="1:11">
+      <c r="L85">
+        <v>11401076.36592</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12">
       <c r="A86" t="s">
         <v>85</v>
       </c>
@@ -4365,8 +4620,11 @@
       <c r="K86">
         <v>5224915.6777</v>
       </c>
-    </row>
-    <row r="87" spans="1:11">
+      <c r="L86">
+        <v>5841361.625</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12">
       <c r="A87" t="s">
         <v>86</v>
       </c>
@@ -4400,8 +4658,11 @@
       <c r="K87">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:11">
+      <c r="L87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12">
       <c r="A88" t="s">
         <v>87</v>
       </c>
@@ -4435,8 +4696,11 @@
       <c r="K88">
         <v>9469352.4868</v>
       </c>
-    </row>
-    <row r="89" spans="1:11">
+      <c r="L88">
+        <v>3126087.1513</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12">
       <c r="A89" t="s">
         <v>88</v>
       </c>
@@ -4470,8 +4734,11 @@
       <c r="K89">
         <v>39203831.6719</v>
       </c>
-    </row>
-    <row r="90" spans="1:11">
+      <c r="L89">
+        <v>45415914.902</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12">
       <c r="A90" t="s">
         <v>89</v>
       </c>
@@ -4505,8 +4772,11 @@
       <c r="K90">
         <v>62080116.548506</v>
       </c>
-    </row>
-    <row r="91" spans="1:11">
+      <c r="L90">
+        <v>74622896.477531</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12">
       <c r="A91" t="s">
         <v>90</v>
       </c>
@@ -4540,8 +4810,11 @@
       <c r="K91">
         <v>3301748.608831</v>
       </c>
-    </row>
-    <row r="92" spans="1:11">
+      <c r="L91">
+        <v>2351353.983856</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12">
       <c r="A92" t="s">
         <v>91</v>
       </c>
@@ -4575,8 +4848,11 @@
       <c r="K92">
         <v>109822596.9457</v>
       </c>
-    </row>
-    <row r="93" spans="1:11">
+      <c r="L92">
+        <v>129570465.5772</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12">
       <c r="A93" t="s">
         <v>92</v>
       </c>
@@ -4610,8 +4886,11 @@
       <c r="K93">
         <v>28755035.9794</v>
       </c>
-    </row>
-    <row r="94" spans="1:11">
+      <c r="L93">
+        <v>30229235.0313</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12">
       <c r="A94" t="s">
         <v>93</v>
       </c>
@@ -4645,8 +4924,11 @@
       <c r="K94">
         <v>14238250.7936</v>
       </c>
-    </row>
-    <row r="95" spans="1:11">
+      <c r="L94">
+        <v>9738590.061100001</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12">
       <c r="A95" t="s">
         <v>94</v>
       </c>
@@ -4680,8 +4962,11 @@
       <c r="K95">
         <v>704596.6709</v>
       </c>
-    </row>
-    <row r="96" spans="1:11">
+      <c r="L95">
+        <v>725576.9198</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12">
       <c r="A96" t="s">
         <v>95</v>
       </c>
@@ -4715,8 +5000,11 @@
       <c r="K96">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:11">
+      <c r="L96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12">
       <c r="A97" t="s">
         <v>96</v>
       </c>
@@ -4750,8 +5038,11 @@
       <c r="K97">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:11">
+      <c r="L97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12">
       <c r="A98" t="s">
         <v>97</v>
       </c>
@@ -4785,8 +5076,11 @@
       <c r="K98">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="1:11">
+      <c r="L98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12">
       <c r="A99" t="s">
         <v>98</v>
       </c>
@@ -4820,8 +5114,11 @@
       <c r="K99">
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="1:11">
+      <c r="L99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12">
       <c r="A100" t="s">
         <v>99</v>
       </c>
@@ -4855,8 +5152,11 @@
       <c r="K100">
         <v>6282181.83845</v>
       </c>
-    </row>
-    <row r="101" spans="1:11">
+      <c r="L100">
+        <v>4600224.37727</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12">
       <c r="A101" t="s">
         <v>100</v>
       </c>
@@ -4890,8 +5190,11 @@
       <c r="K101">
         <v>6204083.9326</v>
       </c>
-    </row>
-    <row r="102" spans="1:11">
+      <c r="L101">
+        <v>7948405.3229</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12">
       <c r="A102" t="s">
         <v>101</v>
       </c>
@@ -4925,8 +5228,11 @@
       <c r="K102">
         <v>2684946.764274</v>
       </c>
-    </row>
-    <row r="103" spans="1:11">
+      <c r="L102">
+        <v>2700412.92177</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12">
       <c r="A103" t="s">
         <v>102</v>
       </c>
@@ -4960,8 +5266,11 @@
       <c r="K103">
         <v>2447962.2071</v>
       </c>
-    </row>
-    <row r="104" spans="1:11">
+      <c r="L103">
+        <v>2701798.4405</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12">
       <c r="A104" t="s">
         <v>103</v>
       </c>
@@ -4995,8 +5304,11 @@
       <c r="K104">
         <v>1121584.8929</v>
       </c>
-    </row>
-    <row r="105" spans="1:11">
+      <c r="L104">
+        <v>1169669.1956</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12">
       <c r="A105" t="s">
         <v>104</v>
       </c>
@@ -5030,8 +5342,11 @@
       <c r="K105">
         <v>2364882.2982</v>
       </c>
-    </row>
-    <row r="106" spans="1:11">
+      <c r="L105">
+        <v>2326031.2242</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12">
       <c r="A106" t="s">
         <v>105</v>
       </c>
@@ -5065,8 +5380,11 @@
       <c r="K106">
         <v>0</v>
       </c>
-    </row>
-    <row r="107" spans="1:11">
+      <c r="L106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12">
       <c r="A107" t="s">
         <v>106</v>
       </c>
@@ -5100,8 +5418,11 @@
       <c r="K107">
         <v>0</v>
       </c>
-    </row>
-    <row r="108" spans="1:11">
+      <c r="L107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12">
       <c r="A108" t="s">
         <v>107</v>
       </c>
@@ -5135,8 +5456,11 @@
       <c r="K108">
         <v>0</v>
       </c>
-    </row>
-    <row r="109" spans="1:11">
+      <c r="L108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12">
       <c r="A109" t="s">
         <v>108</v>
       </c>
@@ -5170,8 +5494,11 @@
       <c r="K109">
         <v>0</v>
       </c>
-    </row>
-    <row r="110" spans="1:11">
+      <c r="L109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12">
       <c r="A110" t="s">
         <v>109</v>
       </c>
@@ -5205,8 +5532,11 @@
       <c r="K110">
         <v>0</v>
       </c>
-    </row>
-    <row r="111" spans="1:11">
+      <c r="L110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12">
       <c r="A111" t="s">
         <v>110</v>
       </c>
@@ -5240,8 +5570,11 @@
       <c r="K111">
         <v>4635420.9816</v>
       </c>
-    </row>
-    <row r="112" spans="1:11">
+      <c r="L111">
+        <v>3068450.4169</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12">
       <c r="A112" t="s">
         <v>111</v>
       </c>
@@ -5275,8 +5608,11 @@
       <c r="K112">
         <v>1047991.245908</v>
       </c>
-    </row>
-    <row r="113" spans="1:11">
+      <c r="L112">
+        <v>1141438.910625</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12">
       <c r="A113" t="s">
         <v>112</v>
       </c>
@@ -5310,8 +5646,11 @@
       <c r="K113">
         <v>77833624.6164</v>
       </c>
-    </row>
-    <row r="114" spans="1:11">
+      <c r="L113">
+        <v>82496041.1107</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12">
       <c r="A114" t="s">
         <v>113</v>
       </c>
@@ -5345,8 +5684,11 @@
       <c r="K114">
         <v>0</v>
       </c>
-    </row>
-    <row r="115" spans="1:11">
+      <c r="L114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12">
       <c r="A115" t="s">
         <v>114</v>
       </c>
@@ -5380,8 +5722,11 @@
       <c r="K115">
         <v>0</v>
       </c>
-    </row>
-    <row r="116" spans="1:11">
+      <c r="L115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12">
       <c r="A116" t="s">
         <v>115</v>
       </c>
@@ -5415,8 +5760,11 @@
       <c r="K116">
         <v>1190135.503139</v>
       </c>
-    </row>
-    <row r="117" spans="1:11">
+      <c r="L116">
+        <v>1166368.326791</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12">
       <c r="A117" t="s">
         <v>116</v>
       </c>
@@ -5450,8 +5798,11 @@
       <c r="K117">
         <v>4243025.9167</v>
       </c>
-    </row>
-    <row r="118" spans="1:11">
+      <c r="L117">
+        <v>4318141.7494</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12">
       <c r="A118" t="s">
         <v>117</v>
       </c>
@@ -5485,8 +5836,11 @@
       <c r="K118">
         <v>2833828.03035</v>
       </c>
-    </row>
-    <row r="119" spans="1:11">
+      <c r="L118">
+        <v>2876955.523636</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12">
       <c r="A119" t="s">
         <v>118</v>
       </c>
@@ -5520,8 +5874,11 @@
       <c r="K119">
         <v>0</v>
       </c>
-    </row>
-    <row r="120" spans="1:11">
+      <c r="L119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12">
       <c r="A120" t="s">
         <v>119</v>
       </c>
@@ -5555,8 +5912,11 @@
       <c r="K120">
         <v>702826468.3257</v>
       </c>
-    </row>
-    <row r="121" spans="1:11">
+      <c r="L120">
+        <v>745576224.5527</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12">
       <c r="A121" t="s">
         <v>120</v>
       </c>
@@ -5590,8 +5950,11 @@
       <c r="K121">
         <v>25175269.5927</v>
       </c>
-    </row>
-    <row r="122" spans="1:11">
+      <c r="L121">
+        <v>24711669.6697</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12">
       <c r="A122" t="s">
         <v>121</v>
       </c>
@@ -5625,8 +5988,11 @@
       <c r="K122">
         <v>3143477.815</v>
       </c>
-    </row>
-    <row r="123" spans="1:11">
+      <c r="L122">
+        <v>3570085.0796</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12">
       <c r="A123" t="s">
         <v>122</v>
       </c>
@@ -5660,8 +6026,11 @@
       <c r="K123">
         <v>21900001.0501</v>
       </c>
-    </row>
-    <row r="124" spans="1:11">
+      <c r="L123">
+        <v>28971751.93</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12">
       <c r="A124" t="s">
         <v>123</v>
       </c>
@@ -5695,8 +6064,11 @@
       <c r="K124">
         <v>2875066.5442</v>
       </c>
-    </row>
-    <row r="125" spans="1:11">
+      <c r="L124">
+        <v>3690120.79502</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12">
       <c r="A125" t="s">
         <v>124</v>
       </c>
@@ -5730,8 +6102,11 @@
       <c r="K125">
         <v>3772346.68123</v>
       </c>
-    </row>
-    <row r="126" spans="1:11">
+      <c r="L125">
+        <v>5406242.1987457</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12">
       <c r="A126" t="s">
         <v>125</v>
       </c>
@@ -5765,8 +6140,11 @@
       <c r="K126">
         <v>1159594.653</v>
       </c>
-    </row>
-    <row r="127" spans="1:11">
+      <c r="L126">
+        <v>958618.767</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12">
       <c r="A127" t="s">
         <v>126</v>
       </c>
@@ -5800,8 +6178,11 @@
       <c r="K127">
         <v>1012431.4711</v>
       </c>
-    </row>
-    <row r="128" spans="1:11">
+      <c r="L127">
+        <v>1787599.843</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12">
       <c r="A128" t="s">
         <v>127</v>
       </c>
@@ -5835,8 +6216,11 @@
       <c r="K128">
         <v>0</v>
       </c>
-    </row>
-    <row r="129" spans="1:11">
+      <c r="L128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12">
       <c r="A129" t="s">
         <v>128</v>
       </c>
@@ -5870,8 +6254,11 @@
       <c r="K129">
         <v>2605705.62957</v>
       </c>
-    </row>
-    <row r="130" spans="1:11">
+      <c r="L129">
+        <v>1979143.716935</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12">
       <c r="A130" t="s">
         <v>129</v>
       </c>
@@ -5905,8 +6292,11 @@
       <c r="K130">
         <v>8346710.23545</v>
       </c>
-    </row>
-    <row r="131" spans="1:11">
+      <c r="L130">
+        <v>6089412.59615</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12">
       <c r="A131" t="s">
         <v>130</v>
       </c>
@@ -5940,8 +6330,11 @@
       <c r="K131">
         <v>3598018.4541</v>
       </c>
-    </row>
-    <row r="132" spans="1:11">
+      <c r="L131">
+        <v>4763682.732</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12">
       <c r="A132" t="s">
         <v>131</v>
       </c>
@@ -5975,8 +6368,11 @@
       <c r="K132">
         <v>1351365.4989</v>
       </c>
-    </row>
-    <row r="133" spans="1:11">
+      <c r="L132">
+        <v>2025684.7303</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12">
       <c r="A133" t="s">
         <v>132</v>
       </c>
@@ -6010,8 +6406,11 @@
       <c r="K133">
         <v>16329539.5511</v>
       </c>
-    </row>
-    <row r="134" spans="1:11">
+      <c r="L133">
+        <v>16615485.3521</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12">
       <c r="A134" t="s">
         <v>133</v>
       </c>
@@ -6045,8 +6444,11 @@
       <c r="K134">
         <v>2962725.6493</v>
       </c>
-    </row>
-    <row r="135" spans="1:11">
+      <c r="L134">
+        <v>2434198.2858</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12">
       <c r="A135" t="s">
         <v>134</v>
       </c>
@@ -6080,8 +6482,11 @@
       <c r="K135">
         <v>27373346.5887</v>
       </c>
-    </row>
-    <row r="136" spans="1:11">
+      <c r="L135">
+        <v>36357911.2387</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12">
       <c r="A136" t="s">
         <v>135</v>
       </c>
@@ -6115,8 +6520,11 @@
       <c r="K136">
         <v>0</v>
       </c>
-    </row>
-    <row r="137" spans="1:11">
+      <c r="L136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:12">
       <c r="A137" t="s">
         <v>136</v>
       </c>
@@ -6150,8 +6558,11 @@
       <c r="K137">
         <v>8157808.5679</v>
       </c>
-    </row>
-    <row r="138" spans="1:11">
+      <c r="L137">
+        <v>9036133.497579999</v>
+      </c>
+    </row>
+    <row r="138" spans="1:12">
       <c r="A138" t="s">
         <v>137</v>
       </c>
@@ -6185,8 +6596,11 @@
       <c r="K138">
         <v>10254189.6245</v>
       </c>
-    </row>
-    <row r="139" spans="1:11">
+      <c r="L138">
+        <v>11761823.1407</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12">
       <c r="A139" t="s">
         <v>138</v>
       </c>
@@ -6220,8 +6634,11 @@
       <c r="K139">
         <v>16477792.6854</v>
       </c>
-    </row>
-    <row r="140" spans="1:11">
+      <c r="L139">
+        <v>12722789.1574</v>
+      </c>
+    </row>
+    <row r="140" spans="1:12">
       <c r="A140" t="s">
         <v>139</v>
       </c>
@@ -6255,8 +6672,11 @@
       <c r="K140">
         <v>5922029.90708</v>
       </c>
-    </row>
-    <row r="141" spans="1:11">
+      <c r="L140">
+        <v>6255158.42493</v>
+      </c>
+    </row>
+    <row r="141" spans="1:12">
       <c r="A141" t="s">
         <v>140</v>
       </c>
@@ -6290,8 +6710,11 @@
       <c r="K141">
         <v>7913144.09685</v>
       </c>
-    </row>
-    <row r="142" spans="1:11">
+      <c r="L141">
+        <v>8346996.92681</v>
+      </c>
+    </row>
+    <row r="142" spans="1:12">
       <c r="A142" t="s">
         <v>141</v>
       </c>
@@ -6325,8 +6748,11 @@
       <c r="K142">
         <v>2478024.43638</v>
       </c>
-    </row>
-    <row r="143" spans="1:11">
+      <c r="L142">
+        <v>2430514.53088</v>
+      </c>
+    </row>
+    <row r="143" spans="1:12">
       <c r="A143" t="s">
         <v>142</v>
       </c>
@@ -6360,8 +6786,11 @@
       <c r="K143">
         <v>973866.18316408</v>
       </c>
-    </row>
-    <row r="144" spans="1:11">
+      <c r="L143">
+        <v>1038358.56116874</v>
+      </c>
+    </row>
+    <row r="144" spans="1:12">
       <c r="A144" t="s">
         <v>143</v>
       </c>
@@ -6395,8 +6824,11 @@
       <c r="K144">
         <v>2579085.589916</v>
       </c>
-    </row>
-    <row r="145" spans="1:11">
+      <c r="L144">
+        <v>3203152.549176</v>
+      </c>
+    </row>
+    <row r="145" spans="1:12">
       <c r="A145" t="s">
         <v>144</v>
       </c>
@@ -6430,8 +6862,11 @@
       <c r="K145">
         <v>1036165.8730313</v>
       </c>
-    </row>
-    <row r="146" spans="1:11">
+      <c r="L145">
+        <v>1207628.7510508</v>
+      </c>
+    </row>
+    <row r="146" spans="1:12">
       <c r="A146" t="s">
         <v>145</v>
       </c>
@@ -6465,8 +6900,11 @@
       <c r="K146">
         <v>3696729.34442</v>
       </c>
-    </row>
-    <row r="147" spans="1:11">
+      <c r="L146">
+        <v>3915280.531392</v>
+      </c>
+    </row>
+    <row r="147" spans="1:12">
       <c r="A147" t="s">
         <v>146</v>
       </c>
@@ -6500,8 +6938,11 @@
       <c r="K147">
         <v>7438942.304635</v>
       </c>
-    </row>
-    <row r="148" spans="1:11">
+      <c r="L147">
+        <v>6455862.191562</v>
+      </c>
+    </row>
+    <row r="148" spans="1:12">
       <c r="A148" t="s">
         <v>147</v>
       </c>
@@ -6535,8 +6976,11 @@
       <c r="K148">
         <v>6385874.6277</v>
       </c>
-    </row>
-    <row r="149" spans="1:11">
+      <c r="L148">
+        <v>6517742.4661</v>
+      </c>
+    </row>
+    <row r="149" spans="1:12">
       <c r="A149" t="s">
         <v>148</v>
       </c>
@@ -6570,8 +7014,11 @@
       <c r="K149">
         <v>30775882.5666</v>
       </c>
-    </row>
-    <row r="150" spans="1:11">
+      <c r="L149">
+        <v>33922885.2975</v>
+      </c>
+    </row>
+    <row r="150" spans="1:12">
       <c r="A150" t="s">
         <v>149</v>
       </c>
@@ -6605,8 +7052,11 @@
       <c r="K150">
         <v>6695818.2071</v>
       </c>
-    </row>
-    <row r="151" spans="1:11">
+      <c r="L150">
+        <v>7039048.7213</v>
+      </c>
+    </row>
+    <row r="151" spans="1:12">
       <c r="A151" t="s">
         <v>150</v>
       </c>
@@ -6640,8 +7090,11 @@
       <c r="K151">
         <v>0</v>
       </c>
-    </row>
-    <row r="152" spans="1:11">
+      <c r="L151">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:12">
       <c r="A152" t="s">
         <v>151</v>
       </c>
@@ -6675,8 +7128,11 @@
       <c r="K152">
         <v>815295.5638</v>
       </c>
-    </row>
-    <row r="153" spans="1:11">
+      <c r="L152">
+        <v>723737.0541</v>
+      </c>
+    </row>
+    <row r="153" spans="1:12">
       <c r="A153" t="s">
         <v>152</v>
       </c>
@@ -6710,8 +7166,11 @@
       <c r="K153">
         <v>3570444.7183</v>
       </c>
-    </row>
-    <row r="154" spans="1:11">
+      <c r="L153">
+        <v>4063679.6412</v>
+      </c>
+    </row>
+    <row r="154" spans="1:12">
       <c r="A154" t="s">
         <v>153</v>
       </c>
@@ -6745,8 +7204,11 @@
       <c r="K154">
         <v>2651865.1254</v>
       </c>
-    </row>
-    <row r="155" spans="1:11">
+      <c r="L154">
+        <v>2685075.2186</v>
+      </c>
+    </row>
+    <row r="155" spans="1:12">
       <c r="A155" t="s">
         <v>154</v>
       </c>
@@ -6780,8 +7242,11 @@
       <c r="K155">
         <v>2035451.121032</v>
       </c>
-    </row>
-    <row r="156" spans="1:11">
+      <c r="L155">
+        <v>2457763.354712</v>
+      </c>
+    </row>
+    <row r="156" spans="1:12">
       <c r="A156" t="s">
         <v>155</v>
       </c>
@@ -6815,8 +7280,11 @@
       <c r="K156">
         <v>8891784.043084599</v>
       </c>
-    </row>
-    <row r="157" spans="1:11">
+      <c r="L156">
+        <v>9813453.866749801</v>
+      </c>
+    </row>
+    <row r="157" spans="1:12">
       <c r="A157" t="s">
         <v>156</v>
       </c>
@@ -6850,8 +7318,11 @@
       <c r="K157">
         <v>4142987.76147</v>
       </c>
-    </row>
-    <row r="158" spans="1:11">
+      <c r="L157">
+        <v>4431559.92548</v>
+      </c>
+    </row>
+    <row r="158" spans="1:12">
       <c r="A158" t="s">
         <v>157</v>
       </c>
@@ -6885,8 +7356,11 @@
       <c r="K158">
         <v>8216712.9807</v>
       </c>
-    </row>
-    <row r="159" spans="1:11">
+      <c r="L158">
+        <v>9166972.296700001</v>
+      </c>
+    </row>
+    <row r="159" spans="1:12">
       <c r="A159" t="s">
         <v>158</v>
       </c>
@@ -6920,8 +7394,11 @@
       <c r="K159">
         <v>17919324.3534</v>
       </c>
-    </row>
-    <row r="160" spans="1:11">
+      <c r="L159">
+        <v>23450941.3417</v>
+      </c>
+    </row>
+    <row r="160" spans="1:12">
       <c r="A160" t="s">
         <v>159</v>
       </c>
@@ -6955,8 +7432,11 @@
       <c r="K160">
         <v>8326793.6534803</v>
       </c>
-    </row>
-    <row r="161" spans="1:11">
+      <c r="L160">
+        <v>10981888.3378533</v>
+      </c>
+    </row>
+    <row r="161" spans="1:12">
       <c r="A161" t="s">
         <v>160</v>
       </c>
@@ -6990,8 +7470,11 @@
       <c r="K161">
         <v>3855407.9528</v>
       </c>
-    </row>
-    <row r="162" spans="1:11">
+      <c r="L161">
+        <v>3250223.5942</v>
+      </c>
+    </row>
+    <row r="162" spans="1:12">
       <c r="A162" t="s">
         <v>161</v>
       </c>
@@ -7025,8 +7508,11 @@
       <c r="K162">
         <v>5073959.6827</v>
       </c>
-    </row>
-    <row r="163" spans="1:11">
+      <c r="L162">
+        <v>3857111.2975</v>
+      </c>
+    </row>
+    <row r="163" spans="1:12">
       <c r="A163" t="s">
         <v>162</v>
       </c>
@@ -7060,8 +7546,11 @@
       <c r="K163">
         <v>3428443.823306</v>
       </c>
-    </row>
-    <row r="164" spans="1:11">
+      <c r="L163">
+        <v>2289731.450572</v>
+      </c>
+    </row>
+    <row r="164" spans="1:12">
       <c r="A164" t="s">
         <v>163</v>
       </c>
@@ -7095,8 +7584,11 @@
       <c r="K164">
         <v>12837323.5316</v>
       </c>
-    </row>
-    <row r="165" spans="1:11">
+      <c r="L164">
+        <v>15189403.1187</v>
+      </c>
+    </row>
+    <row r="165" spans="1:12">
       <c r="A165" t="s">
         <v>164</v>
       </c>
@@ -7130,8 +7622,11 @@
       <c r="K165">
         <v>1569654.468749</v>
       </c>
-    </row>
-    <row r="166" spans="1:11">
+      <c r="L165">
+        <v>1919593.918845</v>
+      </c>
+    </row>
+    <row r="166" spans="1:12">
       <c r="A166" t="s">
         <v>165</v>
       </c>
@@ -7165,8 +7660,11 @@
       <c r="K166">
         <v>77050952.69750001</v>
       </c>
-    </row>
-    <row r="167" spans="1:11">
+      <c r="L166">
+        <v>63792815.8659</v>
+      </c>
+    </row>
+    <row r="167" spans="1:12">
       <c r="A167" t="s">
         <v>166</v>
       </c>
@@ -7200,8 +7698,11 @@
       <c r="K167">
         <v>2412509.7396</v>
       </c>
-    </row>
-    <row r="168" spans="1:11">
+      <c r="L167">
+        <v>1712373.5228</v>
+      </c>
+    </row>
+    <row r="168" spans="1:12">
       <c r="A168" t="s">
         <v>167</v>
       </c>
@@ -7235,8 +7736,11 @@
       <c r="K168">
         <v>60758690.9478</v>
       </c>
-    </row>
-    <row r="169" spans="1:11">
+      <c r="L168">
+        <v>82310751.52779999</v>
+      </c>
+    </row>
+    <row r="169" spans="1:12">
       <c r="A169" t="s">
         <v>168</v>
       </c>
@@ -7270,8 +7774,11 @@
       <c r="K169">
         <v>28272965.7434</v>
       </c>
-    </row>
-    <row r="170" spans="1:11">
+      <c r="L169">
+        <v>56275327.3689</v>
+      </c>
+    </row>
+    <row r="170" spans="1:12">
       <c r="A170" t="s">
         <v>169</v>
       </c>
@@ -7305,8 +7812,11 @@
       <c r="K170">
         <v>6263622.5981</v>
       </c>
-    </row>
-    <row r="171" spans="1:11">
+      <c r="L170">
+        <v>6687934.0092</v>
+      </c>
+    </row>
+    <row r="171" spans="1:12">
       <c r="A171" t="s">
         <v>170</v>
       </c>
@@ -7340,8 +7850,11 @@
       <c r="K171">
         <v>786784.6034</v>
       </c>
-    </row>
-    <row r="172" spans="1:11">
+      <c r="L171">
+        <v>1096378.2091</v>
+      </c>
+    </row>
+    <row r="172" spans="1:12">
       <c r="A172" t="s">
         <v>171</v>
       </c>
@@ -7375,8 +7888,11 @@
       <c r="K172">
         <v>240160739.7861</v>
       </c>
-    </row>
-    <row r="173" spans="1:11">
+      <c r="L172">
+        <v>255352145.7784</v>
+      </c>
+    </row>
+    <row r="173" spans="1:12">
       <c r="A173" t="s">
         <v>172</v>
       </c>
@@ -7410,8 +7926,11 @@
       <c r="K173">
         <v>500977869.185798</v>
       </c>
-    </row>
-    <row r="174" spans="1:11">
+      <c r="L173">
+        <v>398788093.1473</v>
+      </c>
+    </row>
+    <row r="174" spans="1:12">
       <c r="A174" t="s">
         <v>173</v>
       </c>
@@ -7445,8 +7964,11 @@
       <c r="K174">
         <v>11820788.772438</v>
       </c>
-    </row>
-    <row r="175" spans="1:11">
+      <c r="L174">
+        <v>14130676.430689</v>
+      </c>
+    </row>
+    <row r="175" spans="1:12">
       <c r="A175" t="s">
         <v>174</v>
       </c>
@@ -7480,8 +8002,11 @@
       <c r="K175">
         <v>1773187.3737</v>
       </c>
-    </row>
-    <row r="176" spans="1:11">
+      <c r="L175">
+        <v>1832183.6288</v>
+      </c>
+    </row>
+    <row r="176" spans="1:12">
       <c r="A176" t="s">
         <v>175</v>
       </c>
@@ -7515,8 +8040,11 @@
       <c r="K176">
         <v>1548308.7188</v>
       </c>
-    </row>
-    <row r="177" spans="1:11">
+      <c r="L176">
+        <v>947266.1437</v>
+      </c>
+    </row>
+    <row r="177" spans="1:12">
       <c r="A177" t="s">
         <v>176</v>
       </c>
@@ -7550,8 +8078,11 @@
       <c r="K177">
         <v>6488454.6315</v>
       </c>
-    </row>
-    <row r="178" spans="1:11">
+      <c r="L177">
+        <v>7488415.0248</v>
+      </c>
+    </row>
+    <row r="178" spans="1:12">
       <c r="A178" t="s">
         <v>177</v>
       </c>
@@ -7585,8 +8116,11 @@
       <c r="K178">
         <v>6337274.1562</v>
       </c>
-    </row>
-    <row r="179" spans="1:11">
+      <c r="L178">
+        <v>4546299.3218</v>
+      </c>
+    </row>
+    <row r="179" spans="1:12">
       <c r="A179" t="s">
         <v>178</v>
       </c>
@@ -7620,8 +8154,11 @@
       <c r="K179">
         <v>32015060.2723</v>
       </c>
-    </row>
-    <row r="180" spans="1:11">
+      <c r="L179">
+        <v>32375940.5128</v>
+      </c>
+    </row>
+    <row r="180" spans="1:12">
       <c r="A180" t="s">
         <v>179</v>
       </c>
@@ -7655,8 +8192,11 @@
       <c r="K180">
         <v>3482850.0343</v>
       </c>
-    </row>
-    <row r="181" spans="1:11">
+      <c r="L180">
+        <v>4220522.7033</v>
+      </c>
+    </row>
+    <row r="181" spans="1:12">
       <c r="A181" t="s">
         <v>180</v>
       </c>
@@ -7690,8 +8230,11 @@
       <c r="K181">
         <v>16028115.628</v>
       </c>
-    </row>
-    <row r="182" spans="1:11">
+      <c r="L181">
+        <v>15451581.333</v>
+      </c>
+    </row>
+    <row r="182" spans="1:12">
       <c r="A182" t="s">
         <v>181</v>
       </c>
@@ -7725,8 +8268,11 @@
       <c r="K182">
         <v>52890998.0359</v>
       </c>
-    </row>
-    <row r="183" spans="1:11">
+      <c r="L182">
+        <v>65772505.4866</v>
+      </c>
+    </row>
+    <row r="183" spans="1:12">
       <c r="A183" t="s">
         <v>182</v>
       </c>
@@ -7760,8 +8306,11 @@
       <c r="K183">
         <v>4782364.5996</v>
       </c>
-    </row>
-    <row r="184" spans="1:11">
+      <c r="L183">
+        <v>3796190.9111</v>
+      </c>
+    </row>
+    <row r="184" spans="1:12">
       <c r="A184" t="s">
         <v>183</v>
       </c>
@@ -7795,8 +8344,11 @@
       <c r="K184">
         <v>35761706.0926</v>
       </c>
-    </row>
-    <row r="185" spans="1:11">
+      <c r="L184">
+        <v>34540716.2329</v>
+      </c>
+    </row>
+    <row r="185" spans="1:12">
       <c r="A185" t="s">
         <v>184</v>
       </c>
@@ -7830,8 +8382,11 @@
       <c r="K185">
         <v>2564150.6219</v>
       </c>
-    </row>
-    <row r="186" spans="1:11">
+      <c r="L185">
+        <v>3605247.5098</v>
+      </c>
+    </row>
+    <row r="186" spans="1:12">
       <c r="A186" t="s">
         <v>185</v>
       </c>
@@ -7865,8 +8420,11 @@
       <c r="K186">
         <v>2895710.4993</v>
       </c>
-    </row>
-    <row r="187" spans="1:11">
+      <c r="L186">
+        <v>2985239.891</v>
+      </c>
+    </row>
+    <row r="187" spans="1:12">
       <c r="A187" t="s">
         <v>186</v>
       </c>
@@ -7900,8 +8458,11 @@
       <c r="K187">
         <v>3382985.24705</v>
       </c>
-    </row>
-    <row r="188" spans="1:11">
+      <c r="L187">
+        <v>4064081.238207</v>
+      </c>
+    </row>
+    <row r="188" spans="1:12">
       <c r="A188" t="s">
         <v>187</v>
       </c>
@@ -7935,8 +8496,11 @@
       <c r="K188">
         <v>1846077.25964328</v>
       </c>
-    </row>
-    <row r="189" spans="1:11">
+      <c r="L188">
+        <v>2162634.33519267</v>
+      </c>
+    </row>
+    <row r="189" spans="1:12">
       <c r="A189" t="s">
         <v>188</v>
       </c>
@@ -7970,8 +8534,11 @@
       <c r="K189">
         <v>593746.1967932</v>
       </c>
-    </row>
-    <row r="190" spans="1:11">
+      <c r="L189">
+        <v>625012.7378543</v>
+      </c>
+    </row>
+    <row r="190" spans="1:12">
       <c r="A190" t="s">
         <v>189</v>
       </c>
@@ -8005,8 +8572,11 @@
       <c r="K190">
         <v>168142.19835</v>
       </c>
-    </row>
-    <row r="191" spans="1:11">
+      <c r="L190">
+        <v>163539.6788</v>
+      </c>
+    </row>
+    <row r="191" spans="1:12">
       <c r="A191" t="s">
         <v>190</v>
       </c>
@@ -8040,8 +8610,11 @@
       <c r="K191">
         <v>3771055.561055</v>
       </c>
-    </row>
-    <row r="192" spans="1:11">
+      <c r="L191">
+        <v>3995392.4423</v>
+      </c>
+    </row>
+    <row r="192" spans="1:12">
       <c r="A192" t="s">
         <v>191</v>
       </c>
@@ -8075,8 +8648,11 @@
       <c r="K192">
         <v>2832110.28682406</v>
       </c>
-    </row>
-    <row r="193" spans="1:11">
+      <c r="L192">
+        <v>3182883.63954845</v>
+      </c>
+    </row>
+    <row r="193" spans="1:12">
       <c r="A193" t="s">
         <v>192</v>
       </c>
@@ -8110,8 +8686,11 @@
       <c r="K193">
         <v>6360649.2364</v>
       </c>
-    </row>
-    <row r="194" spans="1:11">
+      <c r="L193">
+        <v>6243680.31259</v>
+      </c>
+    </row>
+    <row r="194" spans="1:12">
       <c r="A194" t="s">
         <v>193</v>
       </c>
@@ -8145,8 +8724,11 @@
       <c r="K194">
         <v>3122708.96659068</v>
       </c>
-    </row>
-    <row r="195" spans="1:11">
+      <c r="L194">
+        <v>3130727.43010112</v>
+      </c>
+    </row>
+    <row r="195" spans="1:12">
       <c r="A195" t="s">
         <v>194</v>
       </c>
@@ -8180,8 +8762,11 @@
       <c r="K195">
         <v>2943976.5318</v>
       </c>
-    </row>
-    <row r="196" spans="1:11">
+      <c r="L195">
+        <v>3270161.1614</v>
+      </c>
+    </row>
+    <row r="196" spans="1:12">
       <c r="A196" t="s">
         <v>195</v>
       </c>
@@ -8215,8 +8800,11 @@
       <c r="K196">
         <v>2325656.1041</v>
       </c>
-    </row>
-    <row r="197" spans="1:11">
+      <c r="L196">
+        <v>2579293.1182</v>
+      </c>
+    </row>
+    <row r="197" spans="1:12">
       <c r="A197" t="s">
         <v>196</v>
       </c>
@@ -8250,8 +8838,11 @@
       <c r="K197">
         <v>833537.18376</v>
       </c>
-    </row>
-    <row r="198" spans="1:11">
+      <c r="L197">
+        <v>874285.76036</v>
+      </c>
+    </row>
+    <row r="198" spans="1:12">
       <c r="A198" t="s">
         <v>197</v>
       </c>
@@ -8285,8 +8876,11 @@
       <c r="K198">
         <v>234328.75468</v>
       </c>
-    </row>
-    <row r="199" spans="1:11">
+      <c r="L198">
+        <v>381248.62099</v>
+      </c>
+    </row>
+    <row r="199" spans="1:12">
       <c r="A199" t="s">
         <v>198</v>
       </c>
@@ -8320,8 +8914,11 @@
       <c r="K199">
         <v>65846584.0155</v>
       </c>
-    </row>
-    <row r="200" spans="1:11">
+      <c r="L199">
+        <v>58492588.1746</v>
+      </c>
+    </row>
+    <row r="200" spans="1:12">
       <c r="A200" t="s">
         <v>199</v>
       </c>
@@ -8355,8 +8952,11 @@
       <c r="K200">
         <v>948795.48604</v>
       </c>
-    </row>
-    <row r="201" spans="1:11">
+      <c r="L200">
+        <v>765844.505346</v>
+      </c>
+    </row>
+    <row r="201" spans="1:12">
       <c r="A201" t="s">
         <v>200</v>
       </c>
@@ -8390,8 +8990,11 @@
       <c r="K201">
         <v>6601376.3713</v>
       </c>
-    </row>
-    <row r="202" spans="1:11">
+      <c r="L201">
+        <v>5270308.379</v>
+      </c>
+    </row>
+    <row r="202" spans="1:12">
       <c r="A202" t="s">
         <v>201</v>
       </c>
@@ -8425,8 +9028,11 @@
       <c r="K202">
         <v>2264399.40893</v>
       </c>
-    </row>
-    <row r="203" spans="1:11">
+      <c r="L202">
+        <v>2159778.82221</v>
+      </c>
+    </row>
+    <row r="203" spans="1:12">
       <c r="A203" t="s">
         <v>202</v>
       </c>
@@ -8460,8 +9066,11 @@
       <c r="K203">
         <v>364861290.0669</v>
       </c>
-    </row>
-    <row r="204" spans="1:11">
+      <c r="L203">
+        <v>292417935.2805</v>
+      </c>
+    </row>
+    <row r="204" spans="1:12">
       <c r="A204" t="s">
         <v>203</v>
       </c>
@@ -8495,8 +9104,11 @@
       <c r="K204">
         <v>16458738.2863</v>
       </c>
-    </row>
-    <row r="205" spans="1:11">
+      <c r="L204">
+        <v>32341953.3356</v>
+      </c>
+    </row>
+    <row r="205" spans="1:12">
       <c r="A205" t="s">
         <v>204</v>
       </c>
@@ -8530,8 +9142,11 @@
       <c r="K205">
         <v>6122077.8401</v>
       </c>
-    </row>
-    <row r="206" spans="1:11">
+      <c r="L205">
+        <v>6510700.7393</v>
+      </c>
+    </row>
+    <row r="206" spans="1:12">
       <c r="A206" t="s">
         <v>205</v>
       </c>
@@ -8565,8 +9180,11 @@
       <c r="K206">
         <v>1718035.58585</v>
       </c>
-    </row>
-    <row r="207" spans="1:11">
+      <c r="L206">
+        <v>1382850.89507</v>
+      </c>
+    </row>
+    <row r="207" spans="1:12">
       <c r="A207" t="s">
         <v>206</v>
       </c>
@@ -8600,8 +9218,11 @@
       <c r="K207">
         <v>1011624.98111</v>
       </c>
-    </row>
-    <row r="208" spans="1:11">
+      <c r="L207">
+        <v>809512.44785</v>
+      </c>
+    </row>
+    <row r="208" spans="1:12">
       <c r="A208" t="s">
         <v>207</v>
       </c>
@@ -8635,8 +9256,11 @@
       <c r="K208">
         <v>8965881.685799999</v>
       </c>
-    </row>
-    <row r="209" spans="1:11">
+      <c r="L208">
+        <v>10237829.3834</v>
+      </c>
+    </row>
+    <row r="209" spans="1:12">
       <c r="A209" t="s">
         <v>208</v>
       </c>
@@ -8670,8 +9294,11 @@
       <c r="K209">
         <v>4441768.8915</v>
       </c>
-    </row>
-    <row r="210" spans="1:11">
+      <c r="L209">
+        <v>3201980.0783</v>
+      </c>
+    </row>
+    <row r="210" spans="1:12">
       <c r="A210" t="s">
         <v>209</v>
       </c>
@@ -8705,8 +9332,11 @@
       <c r="K210">
         <v>7703314.0437</v>
       </c>
-    </row>
-    <row r="211" spans="1:11">
+      <c r="L210">
+        <v>8348221.5707</v>
+      </c>
+    </row>
+    <row r="211" spans="1:12">
       <c r="A211" t="s">
         <v>210</v>
       </c>
@@ -8740,8 +9370,11 @@
       <c r="K211">
         <v>10294393.0953</v>
       </c>
-    </row>
-    <row r="212" spans="1:11">
+      <c r="L211">
+        <v>9480831.3947</v>
+      </c>
+    </row>
+    <row r="212" spans="1:12">
       <c r="A212" t="s">
         <v>211</v>
       </c>
@@ -8775,8 +9408,11 @@
       <c r="K212">
         <v>29105548.8994</v>
       </c>
-    </row>
-    <row r="213" spans="1:11">
+      <c r="L212">
+        <v>35616854.1201</v>
+      </c>
+    </row>
+    <row r="213" spans="1:12">
       <c r="A213" t="s">
         <v>212</v>
       </c>
@@ -8810,8 +9446,11 @@
       <c r="K213">
         <v>87983549.6637</v>
       </c>
-    </row>
-    <row r="214" spans="1:11">
+      <c r="L213">
+        <v>85282939.6987</v>
+      </c>
+    </row>
+    <row r="214" spans="1:12">
       <c r="A214" t="s">
         <v>213</v>
       </c>
@@ -8845,8 +9484,11 @@
       <c r="K214">
         <v>1296522.5177864</v>
       </c>
-    </row>
-    <row r="215" spans="1:11">
+      <c r="L214">
+        <v>1472519.2677395</v>
+      </c>
+    </row>
+    <row r="215" spans="1:12">
       <c r="A215" t="s">
         <v>214</v>
       </c>
@@ -8880,8 +9522,11 @@
       <c r="K215">
         <v>829516.370358</v>
       </c>
-    </row>
-    <row r="216" spans="1:11">
+      <c r="L215">
+        <v>925710.424132</v>
+      </c>
+    </row>
+    <row r="216" spans="1:12">
       <c r="A216" t="s">
         <v>215</v>
       </c>
@@ -8915,8 +9560,11 @@
       <c r="K216">
         <v>288495575.8102</v>
       </c>
-    </row>
-    <row r="217" spans="1:11">
+      <c r="L216">
+        <v>283747456.6166</v>
+      </c>
+    </row>
+    <row r="217" spans="1:12">
       <c r="A217" t="s">
         <v>216</v>
       </c>
@@ -8950,8 +9598,11 @@
       <c r="K217">
         <v>3525395.354156</v>
       </c>
-    </row>
-    <row r="218" spans="1:11">
+      <c r="L217">
+        <v>3373570.355004</v>
+      </c>
+    </row>
+    <row r="218" spans="1:12">
       <c r="A218" t="s">
         <v>217</v>
       </c>
@@ -8985,8 +9636,11 @@
       <c r="K218">
         <v>2639331.16699429</v>
       </c>
-    </row>
-    <row r="219" spans="1:11">
+      <c r="L218">
+        <v>2732097.62321451</v>
+      </c>
+    </row>
+    <row r="219" spans="1:12">
       <c r="A219" t="s">
         <v>218</v>
       </c>
@@ -9020,8 +9674,11 @@
       <c r="K219">
         <v>313930.545109</v>
       </c>
-    </row>
-    <row r="220" spans="1:11">
+      <c r="L219">
+        <v>419451.973767</v>
+      </c>
+    </row>
+    <row r="220" spans="1:12">
       <c r="A220" t="s">
         <v>219</v>
       </c>
@@ -9055,8 +9712,11 @@
       <c r="K220">
         <v>142767.152399</v>
       </c>
-    </row>
-    <row r="221" spans="1:11">
+      <c r="L220">
+        <v>217358.520304</v>
+      </c>
+    </row>
+    <row r="221" spans="1:12">
       <c r="A221" t="s">
         <v>220</v>
       </c>
@@ -9090,8 +9750,11 @@
       <c r="K221">
         <v>4038496.5716</v>
       </c>
-    </row>
-    <row r="222" spans="1:11">
+      <c r="L221">
+        <v>7864224.327</v>
+      </c>
+    </row>
+    <row r="222" spans="1:12">
       <c r="A222" t="s">
         <v>221</v>
       </c>
@@ -9125,8 +9788,11 @@
       <c r="K222">
         <v>19461503.3054</v>
       </c>
-    </row>
-    <row r="223" spans="1:11">
+      <c r="L222">
+        <v>20290721.9951</v>
+      </c>
+    </row>
+    <row r="223" spans="1:12">
       <c r="A223" t="s">
         <v>222</v>
       </c>
@@ -9160,8 +9826,11 @@
       <c r="K223">
         <v>9664024.066199999</v>
       </c>
-    </row>
-    <row r="224" spans="1:11">
+      <c r="L223">
+        <v>8768487.4714</v>
+      </c>
+    </row>
+    <row r="224" spans="1:12">
       <c r="A224" t="s">
         <v>223</v>
       </c>
@@ -9195,8 +9864,11 @@
       <c r="K224">
         <v>366336.561353</v>
       </c>
-    </row>
-    <row r="225" spans="1:11">
+      <c r="L224">
+        <v>400232.244376</v>
+      </c>
+    </row>
+    <row r="225" spans="1:12">
       <c r="A225" t="s">
         <v>224</v>
       </c>
@@ -9230,8 +9902,11 @@
       <c r="K225">
         <v>163738.88901</v>
       </c>
-    </row>
-    <row r="226" spans="1:11">
+      <c r="L225">
+        <v>180923.694293</v>
+      </c>
+    </row>
+    <row r="226" spans="1:12">
       <c r="A226" t="s">
         <v>225</v>
       </c>
@@ -9265,8 +9940,11 @@
       <c r="K226">
         <v>4818136.18354</v>
       </c>
-    </row>
-    <row r="227" spans="1:11">
+      <c r="L226">
+        <v>3992494.98248</v>
+      </c>
+    </row>
+    <row r="227" spans="1:12">
       <c r="A227" t="s">
         <v>226</v>
       </c>
@@ -9300,8 +9978,11 @@
       <c r="K227">
         <v>505943422.487466</v>
       </c>
-    </row>
-    <row r="228" spans="1:11">
+      <c r="L227">
+        <v>805427651.808547</v>
+      </c>
+    </row>
+    <row r="228" spans="1:12">
       <c r="A228" t="s">
         <v>227</v>
       </c>
@@ -9335,8 +10016,11 @@
       <c r="K228">
         <v>3240096.8343</v>
       </c>
-    </row>
-    <row r="229" spans="1:11">
+      <c r="L228">
+        <v>2971412.3176</v>
+      </c>
+    </row>
+    <row r="229" spans="1:12">
       <c r="A229" t="s">
         <v>228</v>
       </c>
@@ -9370,8 +10054,11 @@
       <c r="K229">
         <v>3135072.814</v>
       </c>
-    </row>
-    <row r="230" spans="1:11">
+      <c r="L229">
+        <v>3430556.4347</v>
+      </c>
+    </row>
+    <row r="230" spans="1:12">
       <c r="A230" t="s">
         <v>229</v>
       </c>
@@ -9405,8 +10092,11 @@
       <c r="K230">
         <v>2355216.6999</v>
       </c>
-    </row>
-    <row r="231" spans="1:11">
+      <c r="L230">
+        <v>3123675.4983</v>
+      </c>
+    </row>
+    <row r="231" spans="1:12">
       <c r="A231" t="s">
         <v>230</v>
       </c>
@@ -9440,8 +10130,11 @@
       <c r="K231">
         <v>8200515.6886</v>
       </c>
-    </row>
-    <row r="232" spans="1:11">
+      <c r="L231">
+        <v>7481565.3693</v>
+      </c>
+    </row>
+    <row r="232" spans="1:12">
       <c r="A232" t="s">
         <v>231</v>
       </c>
@@ -9475,8 +10168,11 @@
       <c r="K232">
         <v>19065723.334427</v>
       </c>
-    </row>
-    <row r="233" spans="1:11">
+      <c r="L232">
+        <v>17492237.860826</v>
+      </c>
+    </row>
+    <row r="233" spans="1:12">
       <c r="A233" t="s">
         <v>232</v>
       </c>
@@ -9510,8 +10206,11 @@
       <c r="K233">
         <v>1850045.1963</v>
       </c>
-    </row>
-    <row r="234" spans="1:11">
+      <c r="L233">
+        <v>2307575.5092</v>
+      </c>
+    </row>
+    <row r="234" spans="1:12">
       <c r="A234" t="s">
         <v>233</v>
       </c>
@@ -9545,8 +10244,11 @@
       <c r="K234">
         <v>7138355.171</v>
       </c>
-    </row>
-    <row r="235" spans="1:11">
+      <c r="L234">
+        <v>7103054.1769</v>
+      </c>
+    </row>
+    <row r="235" spans="1:12">
       <c r="A235" t="s">
         <v>234</v>
       </c>
@@ -9580,8 +10282,11 @@
       <c r="K235">
         <v>1927109.451385</v>
       </c>
-    </row>
-    <row r="236" spans="1:11">
+      <c r="L235">
+        <v>1921905.689967</v>
+      </c>
+    </row>
+    <row r="236" spans="1:12">
       <c r="A236" t="s">
         <v>235</v>
       </c>
@@ -9615,8 +10320,11 @@
       <c r="K236">
         <v>1410880.36560614</v>
       </c>
-    </row>
-    <row r="237" spans="1:11">
+      <c r="L236">
+        <v>1777808.84666441</v>
+      </c>
+    </row>
+    <row r="237" spans="1:12">
       <c r="A237" t="s">
         <v>236</v>
       </c>
@@ -9650,8 +10358,11 @@
       <c r="K237">
         <v>9979103.495300001</v>
       </c>
-    </row>
-    <row r="238" spans="1:11">
+      <c r="L237">
+        <v>11487875.3698</v>
+      </c>
+    </row>
+    <row r="238" spans="1:12">
       <c r="A238" t="s">
         <v>237</v>
       </c>
@@ -9685,8 +10396,11 @@
       <c r="K238">
         <v>79033.9069</v>
       </c>
-    </row>
-    <row r="239" spans="1:11">
+      <c r="L238">
+        <v>112764.1143</v>
+      </c>
+    </row>
+    <row r="239" spans="1:12">
       <c r="A239" t="s">
         <v>238</v>
       </c>
@@ -9720,8 +10434,11 @@
       <c r="K239">
         <v>3705414.2055058</v>
       </c>
-    </row>
-    <row r="240" spans="1:11">
+      <c r="L239">
+        <v>3688212.7203287</v>
+      </c>
+    </row>
+    <row r="240" spans="1:12">
       <c r="A240" t="s">
         <v>239</v>
       </c>
@@ -9755,8 +10472,11 @@
       <c r="K240">
         <v>1396208.39204</v>
       </c>
-    </row>
-    <row r="241" spans="1:11">
+      <c r="L240">
+        <v>1501512.44835</v>
+      </c>
+    </row>
+    <row r="241" spans="1:12">
       <c r="A241" t="s">
         <v>240</v>
       </c>
@@ -9790,8 +10510,11 @@
       <c r="K241">
         <v>986608.7008554999</v>
       </c>
-    </row>
-    <row r="242" spans="1:11">
+      <c r="L241">
+        <v>851263.2878905</v>
+      </c>
+    </row>
+    <row r="242" spans="1:12">
       <c r="A242" t="s">
         <v>241</v>
       </c>
@@ -9825,8 +10548,11 @@
       <c r="K242">
         <v>278013.28556</v>
       </c>
-    </row>
-    <row r="243" spans="1:11">
+      <c r="L242">
+        <v>321878.94511</v>
+      </c>
+    </row>
+    <row r="243" spans="1:12">
       <c r="A243" t="s">
         <v>242</v>
       </c>
@@ -9860,8 +10586,11 @@
       <c r="K243">
         <v>25146215.3451</v>
       </c>
-    </row>
-    <row r="244" spans="1:11">
+      <c r="L243">
+        <v>27272236.4807</v>
+      </c>
+    </row>
+    <row r="244" spans="1:12">
       <c r="A244" t="s">
         <v>243</v>
       </c>
@@ -9895,8 +10624,11 @@
       <c r="K244">
         <v>7581206.7283</v>
       </c>
-    </row>
-    <row r="245" spans="1:11">
+      <c r="L244">
+        <v>2428304.8421</v>
+      </c>
+    </row>
+    <row r="245" spans="1:12">
       <c r="A245" t="s">
         <v>244</v>
       </c>
@@ -9930,8 +10662,11 @@
       <c r="K245">
         <v>4568226.2474</v>
       </c>
-    </row>
-    <row r="246" spans="1:11">
+      <c r="L245">
+        <v>3463254.1995</v>
+      </c>
+    </row>
+    <row r="246" spans="1:12">
       <c r="A246" t="s">
         <v>245</v>
       </c>
@@ -9965,8 +10700,11 @@
       <c r="K246">
         <v>46641499.1361</v>
       </c>
-    </row>
-    <row r="247" spans="1:11">
+      <c r="L246">
+        <v>39095519.5972</v>
+      </c>
+    </row>
+    <row r="247" spans="1:12">
       <c r="A247" t="s">
         <v>246</v>
       </c>
@@ -10000,8 +10738,11 @@
       <c r="K247">
         <v>17919585.2417</v>
       </c>
-    </row>
-    <row r="248" spans="1:11">
+      <c r="L247">
+        <v>14041470.49092</v>
+      </c>
+    </row>
+    <row r="248" spans="1:12">
       <c r="A248" t="s">
         <v>247</v>
       </c>
@@ -10035,8 +10776,11 @@
       <c r="K248">
         <v>12113062.2755</v>
       </c>
-    </row>
-    <row r="249" spans="1:11">
+      <c r="L248">
+        <v>9053141.204299999</v>
+      </c>
+    </row>
+    <row r="249" spans="1:12">
       <c r="A249" t="s">
         <v>248</v>
       </c>
@@ -10070,8 +10814,11 @@
       <c r="K249">
         <v>2197160.327</v>
       </c>
-    </row>
-    <row r="250" spans="1:11">
+      <c r="L249">
+        <v>1420896.4661</v>
+      </c>
+    </row>
+    <row r="250" spans="1:12">
       <c r="A250" t="s">
         <v>249</v>
       </c>
@@ -10105,8 +10852,11 @@
       <c r="K250">
         <v>897537.4025</v>
       </c>
-    </row>
-    <row r="251" spans="1:11">
+      <c r="L250">
+        <v>692207.2959</v>
+      </c>
+    </row>
+    <row r="251" spans="1:12">
       <c r="A251" t="s">
         <v>250</v>
       </c>
@@ -10140,8 +10890,11 @@
       <c r="K251">
         <v>44581519.9066</v>
       </c>
-    </row>
-    <row r="252" spans="1:11">
+      <c r="L251">
+        <v>42212409.9879</v>
+      </c>
+    </row>
+    <row r="252" spans="1:12">
       <c r="A252" t="s">
         <v>251</v>
       </c>
@@ -10175,8 +10928,11 @@
       <c r="K252">
         <v>668401.2821</v>
       </c>
-    </row>
-    <row r="253" spans="1:11">
+      <c r="L252">
+        <v>597346.3363</v>
+      </c>
+    </row>
+    <row r="253" spans="1:12">
       <c r="A253" t="s">
         <v>252</v>
       </c>
@@ -10210,8 +10966,11 @@
       <c r="K253">
         <v>3543156.8093</v>
       </c>
-    </row>
-    <row r="254" spans="1:11">
+      <c r="L253">
+        <v>2004954.9305</v>
+      </c>
+    </row>
+    <row r="254" spans="1:12">
       <c r="A254" t="s">
         <v>253</v>
       </c>
@@ -10245,8 +11004,11 @@
       <c r="K254">
         <v>7248815.0441</v>
       </c>
-    </row>
-    <row r="255" spans="1:11">
+      <c r="L254">
+        <v>3626041.2079</v>
+      </c>
+    </row>
+    <row r="255" spans="1:12">
       <c r="A255" t="s">
         <v>254</v>
       </c>
@@ -10280,8 +11042,11 @@
       <c r="K255">
         <v>7126942.45433</v>
       </c>
-    </row>
-    <row r="256" spans="1:11">
+      <c r="L255">
+        <v>7583849.03685</v>
+      </c>
+    </row>
+    <row r="256" spans="1:12">
       <c r="A256" t="s">
         <v>255</v>
       </c>
@@ -10315,8 +11080,11 @@
       <c r="K256">
         <v>14040694.4521</v>
       </c>
-    </row>
-    <row r="257" spans="1:11">
+      <c r="L256">
+        <v>13945533.9466</v>
+      </c>
+    </row>
+    <row r="257" spans="1:12">
       <c r="A257" t="s">
         <v>256</v>
       </c>
@@ -10350,8 +11118,11 @@
       <c r="K257">
         <v>3966621.8188</v>
       </c>
-    </row>
-    <row r="258" spans="1:11">
+      <c r="L257">
+        <v>4057824.1574</v>
+      </c>
+    </row>
+    <row r="258" spans="1:12">
       <c r="A258" t="s">
         <v>257</v>
       </c>
@@ -10385,8 +11156,11 @@
       <c r="K258">
         <v>7533832.6192</v>
       </c>
-    </row>
-    <row r="259" spans="1:11">
+      <c r="L258">
+        <v>7695877.4148</v>
+      </c>
+    </row>
+    <row r="259" spans="1:12">
       <c r="A259" t="s">
         <v>258</v>
       </c>
@@ -10420,8 +11194,11 @@
       <c r="K259">
         <v>3990580.7204</v>
       </c>
-    </row>
-    <row r="260" spans="1:11">
+      <c r="L259">
+        <v>3745291.2972</v>
+      </c>
+    </row>
+    <row r="260" spans="1:12">
       <c r="A260" t="s">
         <v>259</v>
       </c>
@@ -10455,8 +11232,11 @@
       <c r="K260">
         <v>12189752.8671</v>
       </c>
-    </row>
-    <row r="261" spans="1:11">
+      <c r="L260">
+        <v>11773436.8551</v>
+      </c>
+    </row>
+    <row r="261" spans="1:12">
       <c r="A261" t="s">
         <v>260</v>
       </c>
@@ -10490,8 +11270,11 @@
       <c r="K261">
         <v>38756005.8464</v>
       </c>
-    </row>
-    <row r="262" spans="1:11">
+      <c r="L261">
+        <v>39192461.8062</v>
+      </c>
+    </row>
+    <row r="262" spans="1:12">
       <c r="A262" t="s">
         <v>261</v>
       </c>
@@ -10525,8 +11308,11 @@
       <c r="K262">
         <v>2735318.1173</v>
       </c>
-    </row>
-    <row r="263" spans="1:11">
+      <c r="L262">
+        <v>1690849.6309</v>
+      </c>
+    </row>
+    <row r="263" spans="1:12">
       <c r="A263" t="s">
         <v>262</v>
       </c>
@@ -10560,8 +11346,11 @@
       <c r="K263">
         <v>3394580.343</v>
       </c>
-    </row>
-    <row r="264" spans="1:11">
+      <c r="L263">
+        <v>1573660.2882</v>
+      </c>
+    </row>
+    <row r="264" spans="1:12">
       <c r="A264" t="s">
         <v>263</v>
       </c>
@@ -10595,8 +11384,11 @@
       <c r="K264">
         <v>3807940.0277</v>
       </c>
-    </row>
-    <row r="265" spans="1:11">
+      <c r="L264">
+        <v>2597840.2137</v>
+      </c>
+    </row>
+    <row r="265" spans="1:12">
       <c r="A265" t="s">
         <v>264</v>
       </c>
@@ -10630,8 +11422,11 @@
       <c r="K265">
         <v>6344924.3147</v>
       </c>
-    </row>
-    <row r="266" spans="1:11">
+      <c r="L265">
+        <v>3626450.669</v>
+      </c>
+    </row>
+    <row r="266" spans="1:12">
       <c r="A266" t="s">
         <v>265</v>
       </c>
@@ -10665,8 +11460,11 @@
       <c r="K266">
         <v>60219815.3505399</v>
       </c>
-    </row>
-    <row r="267" spans="1:11">
+      <c r="L266">
+        <v>51081693.120798</v>
+      </c>
+    </row>
+    <row r="267" spans="1:12">
       <c r="A267" t="s">
         <v>266</v>
       </c>
@@ -10700,8 +11498,11 @@
       <c r="K267">
         <v>7288477.2601</v>
       </c>
-    </row>
-    <row r="268" spans="1:11">
+      <c r="L267">
+        <v>4524164.039</v>
+      </c>
+    </row>
+    <row r="268" spans="1:12">
       <c r="A268" t="s">
         <v>267</v>
       </c>
@@ -10735,8 +11536,11 @@
       <c r="K268">
         <v>62685257.0938</v>
       </c>
-    </row>
-    <row r="269" spans="1:11">
+      <c r="L268">
+        <v>98264721.6381</v>
+      </c>
+    </row>
+    <row r="269" spans="1:12">
       <c r="A269" t="s">
         <v>268</v>
       </c>
@@ -10770,8 +11574,11 @@
       <c r="K269">
         <v>15914964.1392994</v>
       </c>
-    </row>
-    <row r="270" spans="1:11">
+      <c r="L269">
+        <v>12116851.862408</v>
+      </c>
+    </row>
+    <row r="270" spans="1:12">
       <c r="A270" t="s">
         <v>269</v>
       </c>
@@ -10805,8 +11612,11 @@
       <c r="K270">
         <v>10348166.2848</v>
       </c>
-    </row>
-    <row r="271" spans="1:11">
+      <c r="L270">
+        <v>15440694.2625</v>
+      </c>
+    </row>
+    <row r="271" spans="1:12">
       <c r="A271" t="s">
         <v>270</v>
       </c>
@@ -10840,8 +11650,11 @@
       <c r="K271">
         <v>2486311.4607</v>
       </c>
-    </row>
-    <row r="272" spans="1:11">
+      <c r="L271">
+        <v>2691524.8197</v>
+      </c>
+    </row>
+    <row r="272" spans="1:12">
       <c r="A272" t="s">
         <v>271</v>
       </c>
@@ -10875,8 +11688,11 @@
       <c r="K272">
         <v>8289004.6993</v>
       </c>
-    </row>
-    <row r="273" spans="1:11">
+      <c r="L272">
+        <v>7016394.4019</v>
+      </c>
+    </row>
+    <row r="273" spans="1:12">
       <c r="A273" t="s">
         <v>272</v>
       </c>
@@ -10910,8 +11726,11 @@
       <c r="K273">
         <v>24830256.1765</v>
       </c>
-    </row>
-    <row r="274" spans="1:11">
+      <c r="L273">
+        <v>28522582.828</v>
+      </c>
+    </row>
+    <row r="274" spans="1:12">
       <c r="A274" t="s">
         <v>273</v>
       </c>
@@ -10945,8 +11764,11 @@
       <c r="K274">
         <v>15640469.9228</v>
       </c>
-    </row>
-    <row r="275" spans="1:11">
+      <c r="L274">
+        <v>19636200.7546</v>
+      </c>
+    </row>
+    <row r="275" spans="1:12">
       <c r="A275" t="s">
         <v>274</v>
       </c>
@@ -10980,8 +11802,11 @@
       <c r="K275">
         <v>1697841.7024</v>
       </c>
-    </row>
-    <row r="276" spans="1:11">
+      <c r="L275">
+        <v>2245114.9689</v>
+      </c>
+    </row>
+    <row r="276" spans="1:12">
       <c r="A276" t="s">
         <v>275</v>
       </c>
@@ -11015,8 +11840,11 @@
       <c r="K276">
         <v>7985348.0642</v>
       </c>
-    </row>
-    <row r="277" spans="1:11">
+      <c r="L276">
+        <v>10646809.1237</v>
+      </c>
+    </row>
+    <row r="277" spans="1:12">
       <c r="A277" t="s">
         <v>276</v>
       </c>
@@ -11050,8 +11878,11 @@
       <c r="K277">
         <v>4596784.7236</v>
       </c>
-    </row>
-    <row r="278" spans="1:11">
+      <c r="L277">
+        <v>3313175.6808</v>
+      </c>
+    </row>
+    <row r="278" spans="1:12">
       <c r="A278" t="s">
         <v>277</v>
       </c>
@@ -11085,8 +11916,11 @@
       <c r="K278">
         <v>39187561.3453</v>
       </c>
-    </row>
-    <row r="279" spans="1:11">
+      <c r="L278">
+        <v>40758644.2539</v>
+      </c>
+    </row>
+    <row r="279" spans="1:12">
       <c r="A279" t="s">
         <v>278</v>
       </c>
@@ -11120,8 +11954,11 @@
       <c r="K279">
         <v>2868221.57754447</v>
       </c>
-    </row>
-    <row r="280" spans="1:11">
+      <c r="L279">
+        <v>1895566.61657187</v>
+      </c>
+    </row>
+    <row r="280" spans="1:12">
       <c r="A280" t="s">
         <v>279</v>
       </c>
@@ -11155,8 +11992,11 @@
       <c r="K280">
         <v>2214260.1665473</v>
       </c>
-    </row>
-    <row r="281" spans="1:11">
+      <c r="L280">
+        <v>1452166.5859241</v>
+      </c>
+    </row>
+    <row r="281" spans="1:12">
       <c r="A281" t="s">
         <v>280</v>
       </c>
@@ -11190,8 +12030,11 @@
       <c r="K281">
         <v>571032.0977</v>
       </c>
-    </row>
-    <row r="282" spans="1:11">
+      <c r="L281">
+        <v>663787.9238</v>
+      </c>
+    </row>
+    <row r="282" spans="1:12">
       <c r="A282" t="s">
         <v>281</v>
       </c>
@@ -11225,8 +12068,11 @@
       <c r="K282">
         <v>3429512.9434</v>
       </c>
-    </row>
-    <row r="283" spans="1:11">
+      <c r="L282">
+        <v>2339733.6562</v>
+      </c>
+    </row>
+    <row r="283" spans="1:12">
       <c r="A283" t="s">
         <v>282</v>
       </c>
@@ -11260,8 +12106,11 @@
       <c r="K283">
         <v>3634938.6639</v>
       </c>
-    </row>
-    <row r="284" spans="1:11">
+      <c r="L283">
+        <v>1230713.0817</v>
+      </c>
+    </row>
+    <row r="284" spans="1:12">
       <c r="A284" t="s">
         <v>283</v>
       </c>
@@ -11295,8 +12144,11 @@
       <c r="K284">
         <v>2646178.1022</v>
       </c>
-    </row>
-    <row r="285" spans="1:11">
+      <c r="L284">
+        <v>2770655.4729</v>
+      </c>
+    </row>
+    <row r="285" spans="1:12">
       <c r="A285" t="s">
         <v>284</v>
       </c>
@@ -11330,8 +12182,11 @@
       <c r="K285">
         <v>15677934.2606</v>
       </c>
-    </row>
-    <row r="286" spans="1:11">
+      <c r="L285">
+        <v>14540393.6402</v>
+      </c>
+    </row>
+    <row r="286" spans="1:12">
       <c r="A286" t="s">
         <v>285</v>
       </c>
@@ -11365,8 +12220,11 @@
       <c r="K286">
         <v>2063182.6345</v>
       </c>
-    </row>
-    <row r="287" spans="1:11">
+      <c r="L286">
+        <v>2412843.558</v>
+      </c>
+    </row>
+    <row r="287" spans="1:12">
       <c r="A287" t="s">
         <v>286</v>
       </c>
@@ -11400,8 +12258,11 @@
       <c r="K287">
         <v>78198666.3777</v>
       </c>
-    </row>
-    <row r="288" spans="1:11">
+      <c r="L287">
+        <v>194807477.5932</v>
+      </c>
+    </row>
+    <row r="288" spans="1:12">
       <c r="A288" t="s">
         <v>287</v>
       </c>
@@ -11435,8 +12296,11 @@
       <c r="K288">
         <v>140420024.0716188</v>
       </c>
-    </row>
-    <row r="289" spans="1:11">
+      <c r="L288">
+        <v>185241487.5482138</v>
+      </c>
+    </row>
+    <row r="289" spans="1:12">
       <c r="A289" t="s">
         <v>288</v>
       </c>
@@ -11470,8 +12334,11 @@
       <c r="K289">
         <v>65546158.1718</v>
       </c>
-    </row>
-    <row r="290" spans="1:11">
+      <c r="L289">
+        <v>63192877.4772</v>
+      </c>
+    </row>
+    <row r="290" spans="1:12">
       <c r="A290" t="s">
         <v>289</v>
       </c>
@@ -11505,8 +12372,11 @@
       <c r="K290">
         <v>45279233.624</v>
       </c>
-    </row>
-    <row r="291" spans="1:11">
+      <c r="L290">
+        <v>23774215.5714</v>
+      </c>
+    </row>
+    <row r="291" spans="1:12">
       <c r="A291" t="s">
         <v>290</v>
       </c>
@@ -11540,8 +12410,11 @@
       <c r="K291">
         <v>6700336.2064</v>
       </c>
-    </row>
-    <row r="292" spans="1:11">
+      <c r="L291">
+        <v>2474813.0273</v>
+      </c>
+    </row>
+    <row r="292" spans="1:12">
       <c r="A292" t="s">
         <v>291</v>
       </c>
@@ -11575,8 +12448,11 @@
       <c r="K292">
         <v>10550908.1924</v>
       </c>
-    </row>
-    <row r="293" spans="1:11">
+      <c r="L292">
+        <v>7419323.5986</v>
+      </c>
+    </row>
+    <row r="293" spans="1:12">
       <c r="A293" t="s">
         <v>292</v>
       </c>
@@ -11610,8 +12486,11 @@
       <c r="K293">
         <v>18390241.9056</v>
       </c>
-    </row>
-    <row r="294" spans="1:11">
+      <c r="L293">
+        <v>16680857.121</v>
+      </c>
+    </row>
+    <row r="294" spans="1:12">
       <c r="A294" t="s">
         <v>293</v>
       </c>
@@ -11645,8 +12524,11 @@
       <c r="K294">
         <v>1630253.1647</v>
       </c>
-    </row>
-    <row r="295" spans="1:11">
+      <c r="L294">
+        <v>1127553.5021</v>
+      </c>
+    </row>
+    <row r="295" spans="1:12">
       <c r="A295" t="s">
         <v>294</v>
       </c>
@@ -11680,8 +12562,11 @@
       <c r="K295">
         <v>3452878.8212</v>
       </c>
-    </row>
-    <row r="296" spans="1:11">
+      <c r="L295">
+        <v>2359684.345</v>
+      </c>
+    </row>
+    <row r="296" spans="1:12">
       <c r="A296" t="s">
         <v>295</v>
       </c>
@@ -11715,8 +12600,11 @@
       <c r="K296">
         <v>2813050.08255</v>
       </c>
-    </row>
-    <row r="297" spans="1:11">
+      <c r="L296">
+        <v>3197249.08042</v>
+      </c>
+    </row>
+    <row r="297" spans="1:12">
       <c r="A297" t="s">
         <v>296</v>
       </c>
@@ -11750,8 +12638,11 @@
       <c r="K297">
         <v>36183542.2113</v>
       </c>
-    </row>
-    <row r="298" spans="1:11">
+      <c r="L297">
+        <v>40145907.0121</v>
+      </c>
+    </row>
+    <row r="298" spans="1:12">
       <c r="A298" t="s">
         <v>297</v>
       </c>
@@ -11785,8 +12676,11 @@
       <c r="K298">
         <v>6385470.2054</v>
       </c>
-    </row>
-    <row r="299" spans="1:11">
+      <c r="L298">
+        <v>7776074.7631</v>
+      </c>
+    </row>
+    <row r="299" spans="1:12">
       <c r="A299" t="s">
         <v>298</v>
       </c>
@@ -11820,8 +12714,11 @@
       <c r="K299">
         <v>2049521.6621</v>
       </c>
-    </row>
-    <row r="300" spans="1:11">
+      <c r="L299">
+        <v>2068802.6408</v>
+      </c>
+    </row>
+    <row r="300" spans="1:12">
       <c r="A300" t="s">
         <v>299</v>
       </c>
@@ -11855,8 +12752,11 @@
       <c r="K300">
         <v>7298725.955</v>
       </c>
-    </row>
-    <row r="301" spans="1:11">
+      <c r="L300">
+        <v>5269602.734</v>
+      </c>
+    </row>
+    <row r="301" spans="1:12">
       <c r="A301" t="s">
         <v>300</v>
       </c>
@@ -11890,8 +12790,11 @@
       <c r="K301">
         <v>4812462.8973</v>
       </c>
-    </row>
-    <row r="302" spans="1:11">
+      <c r="L301">
+        <v>2917097.7807</v>
+      </c>
+    </row>
+    <row r="302" spans="1:12">
       <c r="A302" t="s">
         <v>301</v>
       </c>
@@ -11925,8 +12828,11 @@
       <c r="K302">
         <v>3873257.6555</v>
       </c>
-    </row>
-    <row r="303" spans="1:11">
+      <c r="L302">
+        <v>4441630.4721</v>
+      </c>
+    </row>
+    <row r="303" spans="1:12">
       <c r="A303" t="s">
         <v>302</v>
       </c>
@@ -11960,8 +12866,11 @@
       <c r="K303">
         <v>3938450.5572</v>
       </c>
-    </row>
-    <row r="304" spans="1:11">
+      <c r="L303">
+        <v>3574877.3579</v>
+      </c>
+    </row>
+    <row r="304" spans="1:12">
       <c r="A304" t="s">
         <v>303</v>
       </c>
@@ -11995,8 +12904,11 @@
       <c r="K304">
         <v>1476077.4548</v>
       </c>
-    </row>
-    <row r="305" spans="1:11">
+      <c r="L304">
+        <v>1305840.292</v>
+      </c>
+    </row>
+    <row r="305" spans="1:12">
       <c r="A305" t="s">
         <v>304</v>
       </c>
@@ -12030,8 +12942,11 @@
       <c r="K305">
         <v>2066054.6532</v>
       </c>
-    </row>
-    <row r="306" spans="1:11">
+      <c r="L305">
+        <v>1995756.3089</v>
+      </c>
+    </row>
+    <row r="306" spans="1:12">
       <c r="A306" t="s">
         <v>305</v>
       </c>
@@ -12065,8 +12980,11 @@
       <c r="K306">
         <v>2679152.7302</v>
       </c>
-    </row>
-    <row r="307" spans="1:11">
+      <c r="L306">
+        <v>2716050.1795</v>
+      </c>
+    </row>
+    <row r="307" spans="1:12">
       <c r="A307" t="s">
         <v>306</v>
       </c>
@@ -12100,8 +13018,11 @@
       <c r="K307">
         <v>111611008.7228</v>
       </c>
-    </row>
-    <row r="308" spans="1:11">
+      <c r="L307">
+        <v>87277548.84819999</v>
+      </c>
+    </row>
+    <row r="308" spans="1:12">
       <c r="A308" t="s">
         <v>307</v>
       </c>
@@ -12135,8 +13056,11 @@
       <c r="K308">
         <v>4335558.1112</v>
       </c>
-    </row>
-    <row r="309" spans="1:11">
+      <c r="L308">
+        <v>5496175.6658</v>
+      </c>
+    </row>
+    <row r="309" spans="1:12">
       <c r="A309" t="s">
         <v>308</v>
       </c>
@@ -12170,8 +13094,11 @@
       <c r="K309">
         <v>14719250.8052</v>
       </c>
-    </row>
-    <row r="310" spans="1:11">
+      <c r="L309">
+        <v>11192698.1455</v>
+      </c>
+    </row>
+    <row r="310" spans="1:12">
       <c r="A310" t="s">
         <v>309</v>
       </c>
@@ -12205,8 +13132,11 @@
       <c r="K310">
         <v>6477360.1849</v>
       </c>
-    </row>
-    <row r="311" spans="1:11">
+      <c r="L310">
+        <v>7474443.4569</v>
+      </c>
+    </row>
+    <row r="311" spans="1:12">
       <c r="A311" t="s">
         <v>310</v>
       </c>
@@ -12240,8 +13170,11 @@
       <c r="K311">
         <v>2934508.9463</v>
       </c>
-    </row>
-    <row r="312" spans="1:11">
+      <c r="L311">
+        <v>2907846.5948</v>
+      </c>
+    </row>
+    <row r="312" spans="1:12">
       <c r="A312" t="s">
         <v>311</v>
       </c>
@@ -12275,8 +13208,11 @@
       <c r="K312">
         <v>21815738.902</v>
       </c>
-    </row>
-    <row r="313" spans="1:11">
+      <c r="L312">
+        <v>23071383.4626</v>
+      </c>
+    </row>
+    <row r="313" spans="1:12">
       <c r="A313" t="s">
         <v>312</v>
       </c>
@@ -12310,8 +13246,11 @@
       <c r="K313">
         <v>19801757.7472</v>
       </c>
-    </row>
-    <row r="314" spans="1:11">
+      <c r="L313">
+        <v>15742031.6499</v>
+      </c>
+    </row>
+    <row r="314" spans="1:12">
       <c r="A314" t="s">
         <v>313</v>
       </c>
@@ -12345,8 +13284,11 @@
       <c r="K314">
         <v>3259312.2584</v>
       </c>
-    </row>
-    <row r="315" spans="1:11">
+      <c r="L314">
+        <v>1784852.4554</v>
+      </c>
+    </row>
+    <row r="315" spans="1:12">
       <c r="A315" t="s">
         <v>314</v>
       </c>
@@ -12380,8 +13322,11 @@
       <c r="K315">
         <v>2942550.26099</v>
       </c>
-    </row>
-    <row r="316" spans="1:11">
+      <c r="L315">
+        <v>3045466.46681</v>
+      </c>
+    </row>
+    <row r="316" spans="1:12">
       <c r="A316" t="s">
         <v>315</v>
       </c>
@@ -12415,8 +13360,11 @@
       <c r="K316">
         <v>2311323.5692</v>
       </c>
-    </row>
-    <row r="317" spans="1:11">
+      <c r="L316">
+        <v>1990009.738</v>
+      </c>
+    </row>
+    <row r="317" spans="1:12">
       <c r="A317" t="s">
         <v>316</v>
       </c>
@@ -12450,8 +13398,11 @@
       <c r="K317">
         <v>29466436.4944</v>
       </c>
-    </row>
-    <row r="318" spans="1:11">
+      <c r="L317">
+        <v>27607797.5945</v>
+      </c>
+    </row>
+    <row r="318" spans="1:12">
       <c r="A318" t="s">
         <v>317</v>
       </c>
@@ -12485,8 +13436,11 @@
       <c r="K318">
         <v>16604235.45763</v>
       </c>
-    </row>
-    <row r="319" spans="1:11">
+      <c r="L318">
+        <v>9123190.124539999</v>
+      </c>
+    </row>
+    <row r="319" spans="1:12">
       <c r="A319" t="s">
         <v>318</v>
       </c>
@@ -12520,8 +13474,11 @@
       <c r="K319">
         <v>5338719.0471</v>
       </c>
-    </row>
-    <row r="320" spans="1:11">
+      <c r="L319">
+        <v>1716082.9707</v>
+      </c>
+    </row>
+    <row r="320" spans="1:12">
       <c r="A320" t="s">
         <v>319</v>
       </c>
@@ -12555,8 +13512,11 @@
       <c r="K320">
         <v>628631.2774</v>
       </c>
-    </row>
-    <row r="321" spans="1:11">
+      <c r="L320">
+        <v>829329.6850000001</v>
+      </c>
+    </row>
+    <row r="321" spans="1:12">
       <c r="A321" t="s">
         <v>320</v>
       </c>
@@ -12590,8 +13550,11 @@
       <c r="K321">
         <v>22222859.3795</v>
       </c>
-    </row>
-    <row r="322" spans="1:11">
+      <c r="L321">
+        <v>24296558.293</v>
+      </c>
+    </row>
+    <row r="322" spans="1:12">
       <c r="A322" t="s">
         <v>321</v>
       </c>
@@ -12625,8 +13588,11 @@
       <c r="K322">
         <v>1667951.3716</v>
       </c>
-    </row>
-    <row r="323" spans="1:11">
+      <c r="L322">
+        <v>1641860.5958</v>
+      </c>
+    </row>
+    <row r="323" spans="1:12">
       <c r="A323" t="s">
         <v>322</v>
       </c>
@@ -12660,8 +13626,11 @@
       <c r="K323">
         <v>430703.9279</v>
       </c>
-    </row>
-    <row r="324" spans="1:11">
+      <c r="L323">
+        <v>256207.8081</v>
+      </c>
+    </row>
+    <row r="324" spans="1:12">
       <c r="A324" t="s">
         <v>323</v>
       </c>
@@ -12695,8 +13664,11 @@
       <c r="K324">
         <v>24375172.33444122</v>
       </c>
-    </row>
-    <row r="325" spans="1:11">
+      <c r="L324">
+        <v>21779149.99479388</v>
+      </c>
+    </row>
+    <row r="325" spans="1:12">
       <c r="A325" t="s">
         <v>324</v>
       </c>
@@ -12730,8 +13702,11 @@
       <c r="K325">
         <v>2042667.66929</v>
       </c>
-    </row>
-    <row r="326" spans="1:11">
+      <c r="L325">
+        <v>4624906.98021</v>
+      </c>
+    </row>
+    <row r="326" spans="1:12">
       <c r="A326" t="s">
         <v>325</v>
       </c>
@@ -12765,8 +13740,11 @@
       <c r="K326">
         <v>195692382.81889</v>
       </c>
-    </row>
-    <row r="327" spans="1:11">
+      <c r="L326">
+        <v>315733830.12554</v>
+      </c>
+    </row>
+    <row r="327" spans="1:12">
       <c r="A327" t="s">
         <v>326</v>
       </c>
@@ -12800,8 +13778,11 @@
       <c r="K327">
         <v>15742852.9256</v>
       </c>
-    </row>
-    <row r="328" spans="1:11">
+      <c r="L327">
+        <v>32860552.08982</v>
+      </c>
+    </row>
+    <row r="328" spans="1:12">
       <c r="A328" t="s">
         <v>327</v>
       </c>
@@ -12835,8 +13816,11 @@
       <c r="K328">
         <v>19104120.320622</v>
       </c>
-    </row>
-    <row r="329" spans="1:11">
+      <c r="L328">
+        <v>13956746.112663</v>
+      </c>
+    </row>
+    <row r="329" spans="1:12">
       <c r="A329" t="s">
         <v>328</v>
       </c>
@@ -12870,8 +13854,11 @@
       <c r="K329">
         <v>4950854.26742</v>
       </c>
-    </row>
-    <row r="330" spans="1:11">
+      <c r="L329">
+        <v>4819284.20435</v>
+      </c>
+    </row>
+    <row r="330" spans="1:12">
       <c r="A330" t="s">
         <v>329</v>
       </c>
@@ -12905,8 +13892,11 @@
       <c r="K330">
         <v>1916655.860844</v>
       </c>
-    </row>
-    <row r="331" spans="1:11">
+      <c r="L330">
+        <v>3209664.058851</v>
+      </c>
+    </row>
+    <row r="331" spans="1:12">
       <c r="A331" t="s">
         <v>330</v>
       </c>
@@ -12940,8 +13930,11 @@
       <c r="K331">
         <v>247314651.19214</v>
       </c>
-    </row>
-    <row r="332" spans="1:11">
+      <c r="L331">
+        <v>304996539.35824</v>
+      </c>
+    </row>
+    <row r="332" spans="1:12">
       <c r="A332" t="s">
         <v>331</v>
       </c>
@@ -12975,8 +13968,11 @@
       <c r="K332">
         <v>4019853.6795</v>
       </c>
-    </row>
-    <row r="333" spans="1:11">
+      <c r="L332">
+        <v>4453392.1778</v>
+      </c>
+    </row>
+    <row r="333" spans="1:12">
       <c r="A333" t="s">
         <v>332</v>
       </c>
@@ -13010,8 +14006,11 @@
       <c r="K333">
         <v>27320576.0515</v>
       </c>
-    </row>
-    <row r="334" spans="1:11">
+      <c r="L333">
+        <v>39293817.7335</v>
+      </c>
+    </row>
+    <row r="334" spans="1:12">
       <c r="A334" t="s">
         <v>333</v>
       </c>
@@ -13045,8 +14044,11 @@
       <c r="K334">
         <v>1038992.2449</v>
       </c>
-    </row>
-    <row r="335" spans="1:11">
+      <c r="L334">
+        <v>1081302.2992</v>
+      </c>
+    </row>
+    <row r="335" spans="1:12">
       <c r="A335" t="s">
         <v>334</v>
       </c>
@@ -13079,6 +14081,9 @@
       </c>
       <c r="K335">
         <v>3729888.6684</v>
+      </c>
+      <c r="L335">
+        <v>3273281.9021</v>
       </c>
     </row>
   </sheetData>

</xml_diff>